<commit_message>
Added breakig news and spam files
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/excel.xlsx
+++ b/Aml_automation/src/Common/excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="24240" windowHeight="11025" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="24240" windowHeight="11025" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TagCatagory" sheetId="8" r:id="rId1"/>
@@ -1701,7 +1701,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1921,53 +1921,15 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="37">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment textRotation="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2391,28 +2353,41 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment textRotation="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2426,12 +2401,12 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="13.2"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2618,6 +2593,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -2625,15 +2609,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -2651,11 +2626,11 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="13.2"/>
-        <color theme="1"/>
-        <name val="Arial"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2854,6 +2829,15 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -2861,18 +2845,37 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="13.2"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -2881,51 +2884,51 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E40" totalsRowShown="0" headerRowDxfId="28" headerRowBorderDxfId="35" tableBorderDxfId="36" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E40" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="35" tableBorderDxfId="34" totalsRowBorderDxfId="33">
   <autoFilter ref="A1:E40"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Blog Name" dataDxfId="33"/>
-    <tableColumn id="2" name="Category" dataDxfId="32"/>
-    <tableColumn id="3" name="Tag" dataDxfId="31"/>
-    <tableColumn id="4" name="Club" dataDxfId="30"/>
-    <tableColumn id="5" name="HomepageContent" dataDxfId="29"/>
+    <tableColumn id="1" name="Blog Name" dataDxfId="32"/>
+    <tableColumn id="2" name="Category" dataDxfId="31"/>
+    <tableColumn id="3" name="Tag" dataDxfId="30"/>
+    <tableColumn id="4" name="Club" dataDxfId="29"/>
+    <tableColumn id="5" name="HomepageContent" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="H1:L6" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="26" tableBorderDxfId="27" totalsRowBorderDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="H1:L6" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
   <autoFilter ref="H1:L6"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Image" dataDxfId="24"/>
-    <tableColumn id="2" name="Summary" dataDxfId="23"/>
-    <tableColumn id="3" name="Video" dataDxfId="22"/>
-    <tableColumn id="4" name="Giphy" dataDxfId="21"/>
-    <tableColumn id="5" name="Infogram/Datawrapper" dataDxfId="20"/>
+    <tableColumn id="1" name="Image" dataDxfId="23"/>
+    <tableColumn id="2" name="Summary" dataDxfId="22"/>
+    <tableColumn id="3" name="Video" dataDxfId="21"/>
+    <tableColumn id="4" name="Giphy" dataDxfId="20"/>
+    <tableColumn id="5" name="Infogram/Datawrapper" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:N7" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:N7" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
   <autoFilter ref="A1:N7"/>
   <tableColumns count="14">
-    <tableColumn id="1" name="Table Type" dataDxfId="15"/>
-    <tableColumn id="2" name="Tables" dataDxfId="14"/>
-    <tableColumn id="3" name="Youtube Video" dataDxfId="13" dataCellStyle="Hyperlink"/>
-    <tableColumn id="4" name="Vimeo Youtube" dataDxfId="12" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" name="Vine Youtube" dataDxfId="11"/>
-    <tableColumn id="6" name="Facebook Video" dataDxfId="10" dataCellStyle="Hyperlink"/>
-    <tableColumn id="7" name="Twitter video" dataDxfId="9"/>
-    <tableColumn id="8" name="FB Embed" dataDxfId="8"/>
-    <tableColumn id="9" name="Twitter embed" dataDxfId="7"/>
-    <tableColumn id="10" name="Giphy" dataDxfId="6" dataCellStyle="Hyperlink"/>
-    <tableColumn id="11" name="Infogram" dataDxfId="5" dataCellStyle="Hyperlink"/>
-    <tableColumn id="12" name="Datawrapper" dataDxfId="4" dataCellStyle="Hyperlink"/>
-    <tableColumn id="13" name="Ficha Tecnica" dataDxfId="3"/>
-    <tableColumn id="14" name="Ficha review" dataDxfId="2"/>
+    <tableColumn id="1" name="Table Type" dataDxfId="13"/>
+    <tableColumn id="2" name="Tables" dataDxfId="12"/>
+    <tableColumn id="3" name="Youtube Video" dataDxfId="11" dataCellStyle="Hyperlink"/>
+    <tableColumn id="4" name="Vimeo Youtube" dataDxfId="10" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" name="Vine Youtube" dataDxfId="9"/>
+    <tableColumn id="6" name="Facebook Video" dataDxfId="8" dataCellStyle="Hyperlink"/>
+    <tableColumn id="7" name="Twitter video" dataDxfId="7"/>
+    <tableColumn id="8" name="FB Embed" dataDxfId="6"/>
+    <tableColumn id="9" name="Twitter embed" dataDxfId="5"/>
+    <tableColumn id="10" name="Giphy" dataDxfId="4" dataCellStyle="Hyperlink"/>
+    <tableColumn id="11" name="Infogram" dataDxfId="3" dataCellStyle="Hyperlink"/>
+    <tableColumn id="12" name="Datawrapper" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="13" name="Ficha Tecnica" dataDxfId="1"/>
+    <tableColumn id="14" name="Ficha review" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4051,7 +4054,7 @@
       <c r="K33" s="23"/>
       <c r="L33" s="23"/>
     </row>
-    <row r="34" spans="1:12" ht="39">
+    <row r="34" spans="1:12" ht="26.25">
       <c r="A34" s="36" t="s">
         <v>240</v>
       </c>
@@ -4260,8 +4263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4439,7 +4442,7 @@
       <c r="I4" s="26" t="s">
         <v>352</v>
       </c>
-      <c r="J4" s="61" t="s">
+      <c r="J4" s="77" t="s">
         <v>353</v>
       </c>
       <c r="K4" s="61" t="s">
@@ -4588,27 +4591,27 @@
     <hyperlink ref="C4" r:id="rId15"/>
     <hyperlink ref="D4" r:id="rId16"/>
     <hyperlink ref="F4" r:id="rId17"/>
-    <hyperlink ref="J4" r:id="rId18"/>
-    <hyperlink ref="K4" r:id="rId19"/>
-    <hyperlink ref="L4" r:id="rId20"/>
-    <hyperlink ref="C5" r:id="rId21"/>
-    <hyperlink ref="D5" r:id="rId22"/>
-    <hyperlink ref="F5" r:id="rId23"/>
-    <hyperlink ref="J5" r:id="rId24"/>
-    <hyperlink ref="K5" r:id="rId25"/>
-    <hyperlink ref="L5" r:id="rId26"/>
-    <hyperlink ref="C6" r:id="rId27"/>
-    <hyperlink ref="D6" r:id="rId28"/>
-    <hyperlink ref="F6" r:id="rId29"/>
-    <hyperlink ref="J6" r:id="rId30"/>
-    <hyperlink ref="K6" r:id="rId31"/>
-    <hyperlink ref="L6" r:id="rId32"/>
-    <hyperlink ref="C7" r:id="rId33"/>
-    <hyperlink ref="D7" r:id="rId34"/>
-    <hyperlink ref="F7" r:id="rId35"/>
-    <hyperlink ref="J7" r:id="rId36"/>
-    <hyperlink ref="K7" r:id="rId37"/>
-    <hyperlink ref="L7" r:id="rId38"/>
+    <hyperlink ref="K4" r:id="rId18"/>
+    <hyperlink ref="L4" r:id="rId19"/>
+    <hyperlink ref="C5" r:id="rId20"/>
+    <hyperlink ref="D5" r:id="rId21"/>
+    <hyperlink ref="F5" r:id="rId22"/>
+    <hyperlink ref="J5" r:id="rId23"/>
+    <hyperlink ref="K5" r:id="rId24"/>
+    <hyperlink ref="L5" r:id="rId25"/>
+    <hyperlink ref="C6" r:id="rId26"/>
+    <hyperlink ref="D6" r:id="rId27"/>
+    <hyperlink ref="F6" r:id="rId28"/>
+    <hyperlink ref="J6" r:id="rId29"/>
+    <hyperlink ref="K6" r:id="rId30"/>
+    <hyperlink ref="L6" r:id="rId31"/>
+    <hyperlink ref="C7" r:id="rId32"/>
+    <hyperlink ref="D7" r:id="rId33"/>
+    <hyperlink ref="F7" r:id="rId34"/>
+    <hyperlink ref="J7" r:id="rId35"/>
+    <hyperlink ref="K7" r:id="rId36"/>
+    <hyperlink ref="L7" r:id="rId37"/>
+    <hyperlink ref="J4" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -8445,7 +8448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BY2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Excel Dashboard Button sanity for Unbranded collaborator role
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/excel.xlsx
+++ b/Aml_automation/src/Common/excel.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Agile\Automation\Aml_automation\src\Common\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17535" windowHeight="5400" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17535" windowHeight="5400" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TagCatagory" sheetId="8" r:id="rId1"/>
@@ -22,7 +17,7 @@
     <sheet name="Dashboard TODO Editorial Roles" sheetId="13" r:id="rId8"/>
     <sheet name="Dashboard Programmed Editorial" sheetId="14" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1844,7 +1839,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="20">
     <font>
       <sz val="11"/>
@@ -2845,7 +2840,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2875,7 +2870,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2901,7 +2896,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2928,7 +2923,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2955,7 +2950,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2988,7 +2983,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3020,7 +3015,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3052,7 +3047,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3078,7 +3073,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3111,7 +3106,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3137,7 +3132,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3164,7 +3159,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3197,7 +3192,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3277,7 +3272,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment textRotation="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment textRotation="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0"/>
     </dxf>
     <dxf>
@@ -3305,7 +3300,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3333,7 +3328,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3365,7 +3360,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3399,7 +3394,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3433,7 +3428,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3467,7 +3462,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -3529,7 +3524,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3557,7 +3552,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3589,7 +3584,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3629,7 +3624,7 @@
           <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3669,7 +3664,7 @@
           <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3703,7 +3698,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -3765,7 +3760,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3884,7 +3879,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3916,10 +3911,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3951,7 +3945,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4127,7 +4120,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5196,7 +5189,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5557,7 +5550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BZ15"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
@@ -9158,7 +9151,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Y3"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -9426,7 +9419,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BZ2"/>
   <sheetViews>
     <sheetView topLeftCell="AX1" workbookViewId="0">
@@ -9922,10 +9915,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -9995,7 +9988,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10798,11 +10791,11 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11089,7 +11082,7 @@
         <v>47</v>
       </c>
       <c r="R4" s="98" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="S4" s="98" t="s">
         <v>73</v>
@@ -11344,7 +11337,7 @@
         <v>73</v>
       </c>
       <c r="Q7" s="98" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="R7" s="98" t="s">
         <v>73</v>
@@ -11523,7 +11516,7 @@
         <v>73</v>
       </c>
       <c r="T9" s="110" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="U9" s="110" t="s">
         <v>73</v>
@@ -12033,7 +12026,7 @@
         <v>47</v>
       </c>
       <c r="R15" s="98" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="S15" s="98" t="s">
         <v>73</v>
@@ -12253,7 +12246,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
CMS addHook() - 5 Files modified
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/excel.xlsx
+++ b/Aml_automation/src/Common/excel.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10610"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isha/git/Automation/Aml_automation/src/Common/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AML-1\git\Automation\Aml_automation\src\Common\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7F448820-B788-4A45-9DFF-3FCABAF6A400}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="12440" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="23040" windowHeight="12435" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TagCatagory" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2599" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2615" uniqueCount="599">
   <si>
     <t>Table Type</t>
   </si>
@@ -1784,12 +1783,54 @@
   </si>
   <si>
     <t>En ella encontrarás detalles, ideas y gadgets a partir de 10 euros.</t>
+  </si>
+  <si>
+    <t>Publish_to_homepage_checkbox</t>
+  </si>
+  <si>
+    <t>hook</t>
+  </si>
+  <si>
+    <t>hookCustomerLogo</t>
+  </si>
+  <si>
+    <t>hookCustomerName</t>
+  </si>
+  <si>
+    <t>hookLogoLink</t>
+  </si>
+  <si>
+    <t>hookTextarea</t>
+  </si>
+  <si>
+    <t>hookImage</t>
+  </si>
+  <si>
+    <t>hookButtonText</t>
+  </si>
+  <si>
+    <t>hooklogo.jpeg</t>
+  </si>
+  <si>
+    <t>El Corte Inglés</t>
+  </si>
+  <si>
+    <t>https://www.elcorteingles.es/deportes</t>
+  </si>
+  <si>
+    <t>Esa opción estaba hasta ahora restringida a gráficas de esta familia, pero NVIDIA ha anunciado en la conferencia</t>
+  </si>
+  <si>
+    <t>Más información</t>
+  </si>
+  <si>
+    <t>hookimage.jpeg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="37">
     <font>
       <sz val="10"/>
@@ -2524,7 +2565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2899,6 +2940,21 @@
     <xf numFmtId="0" fontId="14" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3179,7 +3235,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -3187,7 +3243,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:1024" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
@@ -4235,7 +4291,7 @@
       <c r="AMI1" s="25"/>
       <c r="AMJ1" s="25"/>
     </row>
-    <row r="2" spans="1:1024" ht="16">
+    <row r="2" spans="1:1024">
       <c r="A2" s="9" t="s">
         <v>240</v>
       </c>
@@ -4265,7 +4321,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:1024" ht="16">
+    <row r="3" spans="1:1024">
       <c r="A3" s="9" t="s">
         <v>263</v>
       </c>
@@ -4299,7 +4355,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" ht="16">
+    <row r="4" spans="1:1024">
       <c r="A4" s="9" t="s">
         <v>277</v>
       </c>
@@ -4331,7 +4387,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="1:1024" ht="16">
+    <row r="5" spans="1:1024">
       <c r="A5" s="9" t="s">
         <v>286</v>
       </c>
@@ -4359,7 +4415,7 @@
       </c>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="1:1024" ht="16">
+    <row r="6" spans="1:1024">
       <c r="A6" s="9" t="s">
         <v>299</v>
       </c>
@@ -5181,7 +5237,7 @@
       <c r="K38" s="25"/>
       <c r="L38" s="25"/>
     </row>
-    <row r="39" spans="1:12" ht="14">
+    <row r="39" spans="1:12" ht="12.75">
       <c r="A39" s="9" t="s">
         <v>527</v>
       </c>
@@ -5205,7 +5261,7 @@
       <c r="K39" s="25"/>
       <c r="L39" s="25"/>
     </row>
-    <row r="40" spans="1:12" ht="14">
+    <row r="40" spans="1:12" ht="12.75">
       <c r="A40" s="20" t="s">
         <v>531</v>
       </c>
@@ -5235,7 +5291,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -5243,7 +5299,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1" s="94" t="s">
@@ -5389,7 +5445,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -5397,7 +5453,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -5687,51 +5743,51 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="F2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="J2" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="K2" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="L2" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="B3" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="D3" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="F3" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="J3" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="K3" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="L3" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="C4" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="D4" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="F4" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="J4" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="K4" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="L4" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="C5" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="D5" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="F5" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="J5" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="K5" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="L5" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="C6" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="D6" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="F6" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="J6" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="K6" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="L6" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="C7" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="D7" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="F7" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="J7" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="K7" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="L7" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId3"/>
+    <hyperlink ref="F2" r:id="rId4"/>
+    <hyperlink ref="J2" r:id="rId5"/>
+    <hyperlink ref="K2" r:id="rId6"/>
+    <hyperlink ref="L2" r:id="rId7"/>
+    <hyperlink ref="B3" r:id="rId8"/>
+    <hyperlink ref="C3" r:id="rId9"/>
+    <hyperlink ref="D3" r:id="rId10"/>
+    <hyperlink ref="F3" r:id="rId11"/>
+    <hyperlink ref="J3" r:id="rId12"/>
+    <hyperlink ref="K3" r:id="rId13"/>
+    <hyperlink ref="L3" r:id="rId14"/>
+    <hyperlink ref="C4" r:id="rId15"/>
+    <hyperlink ref="D4" r:id="rId16"/>
+    <hyperlink ref="F4" r:id="rId17"/>
+    <hyperlink ref="J4" r:id="rId18"/>
+    <hyperlink ref="K4" r:id="rId19"/>
+    <hyperlink ref="L4" r:id="rId20"/>
+    <hyperlink ref="C5" r:id="rId21"/>
+    <hyperlink ref="D5" r:id="rId22"/>
+    <hyperlink ref="F5" r:id="rId23"/>
+    <hyperlink ref="J5" r:id="rId24"/>
+    <hyperlink ref="K5" r:id="rId25"/>
+    <hyperlink ref="L5" r:id="rId26"/>
+    <hyperlink ref="C6" r:id="rId27"/>
+    <hyperlink ref="D6" r:id="rId28"/>
+    <hyperlink ref="F6" r:id="rId29"/>
+    <hyperlink ref="J6" r:id="rId30"/>
+    <hyperlink ref="K6" r:id="rId31"/>
+    <hyperlink ref="L6" r:id="rId32"/>
+    <hyperlink ref="C7" r:id="rId33"/>
+    <hyperlink ref="D7" r:id="rId34"/>
+    <hyperlink ref="F7" r:id="rId35"/>
+    <hyperlink ref="J7" r:id="rId36"/>
+    <hyperlink ref="K7" r:id="rId37"/>
+    <hyperlink ref="L7" r:id="rId38"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -5739,9 +5795,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:84" ht="14">
+    <row r="1" spans="1:84" ht="12.75">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -5983,7 +6039,7 @@
       <c r="CE1" s="32"/>
       <c r="CF1" s="32"/>
     </row>
-    <row r="2" spans="1:84" ht="14">
+    <row r="2" spans="1:84" ht="12.75">
       <c r="A2" s="33" t="s">
         <v>170</v>
       </c>
@@ -6225,7 +6281,7 @@
       <c r="CE2" s="36"/>
       <c r="CF2" s="36"/>
     </row>
-    <row r="3" spans="1:84" ht="14">
+    <row r="3" spans="1:84" ht="12.75">
       <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
@@ -6707,7 +6763,7 @@
       <c r="CE4" s="36"/>
       <c r="CF4" s="36"/>
     </row>
-    <row r="5" spans="1:84" ht="14">
+    <row r="5" spans="1:84" ht="12.75">
       <c r="A5" s="33" t="s">
         <v>235</v>
       </c>
@@ -6949,7 +7005,7 @@
       <c r="CE5" s="36"/>
       <c r="CF5" s="36"/>
     </row>
-    <row r="6" spans="1:84" ht="14">
+    <row r="6" spans="1:84" ht="12.75">
       <c r="A6" s="41" t="s">
         <v>242</v>
       </c>
@@ -7191,7 +7247,7 @@
       <c r="CE6" s="36"/>
       <c r="CF6" s="36"/>
     </row>
-    <row r="7" spans="1:84" ht="14">
+    <row r="7" spans="1:84" ht="12.75">
       <c r="A7" s="41" t="s">
         <v>250</v>
       </c>
@@ -7433,7 +7489,7 @@
       <c r="CE7" s="36"/>
       <c r="CF7" s="36"/>
     </row>
-    <row r="8" spans="1:84" ht="14">
+    <row r="8" spans="1:84" ht="12.75">
       <c r="A8" s="36" t="s">
         <v>258</v>
       </c>
@@ -7675,7 +7731,7 @@
       <c r="CE8" s="36"/>
       <c r="CF8" s="36"/>
     </row>
-    <row r="9" spans="1:84" ht="14">
+    <row r="9" spans="1:84" ht="12.75">
       <c r="A9" s="36" t="s">
         <v>273</v>
       </c>
@@ -7917,7 +7973,7 @@
       <c r="CE9" s="36"/>
       <c r="CF9" s="36"/>
     </row>
-    <row r="10" spans="1:84" ht="14">
+    <row r="10" spans="1:84" ht="12.75">
       <c r="A10" s="36" t="s">
         <v>284</v>
       </c>
@@ -8159,7 +8215,7 @@
       <c r="CE10" s="36"/>
       <c r="CF10" s="36"/>
     </row>
-    <row r="11" spans="1:84" ht="14">
+    <row r="11" spans="1:84" ht="12.75">
       <c r="A11" s="36" t="s">
         <v>291</v>
       </c>
@@ -8401,7 +8457,7 @@
       <c r="CE11" s="36"/>
       <c r="CF11" s="36"/>
     </row>
-    <row r="12" spans="1:84" ht="14">
+    <row r="12" spans="1:84" ht="12.75">
       <c r="A12" s="36" t="s">
         <v>309</v>
       </c>
@@ -8643,7 +8699,7 @@
       <c r="CE12" s="36"/>
       <c r="CF12" s="36"/>
     </row>
-    <row r="13" spans="1:84" ht="14">
+    <row r="13" spans="1:84" ht="12.75">
       <c r="A13" s="33" t="s">
         <v>316</v>
       </c>
@@ -8885,7 +8941,7 @@
       <c r="CE13" s="36"/>
       <c r="CF13" s="36"/>
     </row>
-    <row r="14" spans="1:84" ht="14">
+    <row r="14" spans="1:84" ht="12.75">
       <c r="A14" s="36" t="s">
         <v>329</v>
       </c>
@@ -9127,7 +9183,7 @@
       <c r="CE14" s="36"/>
       <c r="CF14" s="36"/>
     </row>
-    <row r="15" spans="1:84" ht="14">
+    <row r="15" spans="1:84" ht="12.75">
       <c r="A15" s="33" t="s">
         <v>352</v>
       </c>
@@ -9369,7 +9425,7 @@
       <c r="CE15" s="36"/>
       <c r="CF15" s="36"/>
     </row>
-    <row r="16" spans="1:84" ht="16">
+    <row r="16" spans="1:84" ht="15">
       <c r="A16" s="60" t="s">
         <v>170</v>
       </c>
@@ -9625,45 +9681,45 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="I2" r:id="rId2" location="@lounge.jpg" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="O2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="Q2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="X2" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="AB2" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="F3" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="X3" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="F4" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="U4" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
-    <hyperlink ref="F5" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
-    <hyperlink ref="U5" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
-    <hyperlink ref="F9" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
-    <hyperlink ref="F10" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
-    <hyperlink ref="F11" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
-    <hyperlink ref="F12" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
-    <hyperlink ref="F13" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
-    <hyperlink ref="I13" r:id="rId18" location="@lounge.jpg" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
-    <hyperlink ref="W13" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
-    <hyperlink ref="F14" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
-    <hyperlink ref="X14" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
-    <hyperlink ref="AA14" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
-    <hyperlink ref="AL14" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
-    <hyperlink ref="AN14" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
-    <hyperlink ref="AO14" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
-    <hyperlink ref="AP14" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
-    <hyperlink ref="BA14" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
-    <hyperlink ref="F15" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
-    <hyperlink ref="X15" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
-    <hyperlink ref="Q16" r:id="rId30" location="@lounge.jpg" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
-    <hyperlink ref="BN16" r:id="rId31" location="@Ebay@#@23.50&amp;euro;@###@https://testing.xataka.com@#@Xataka@#@15,670&amp;euro;" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
-    <hyperlink ref="BS16" r:id="rId32" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2" location="@lounge.jpg"/>
+    <hyperlink ref="O2" r:id="rId3"/>
+    <hyperlink ref="Q2" r:id="rId4"/>
+    <hyperlink ref="X2" r:id="rId5"/>
+    <hyperlink ref="AB2" r:id="rId6"/>
+    <hyperlink ref="F3" r:id="rId7"/>
+    <hyperlink ref="X3" r:id="rId8"/>
+    <hyperlink ref="F4" r:id="rId9"/>
+    <hyperlink ref="U4" r:id="rId10"/>
+    <hyperlink ref="F5" r:id="rId11"/>
+    <hyperlink ref="U5" r:id="rId12"/>
+    <hyperlink ref="F9" r:id="rId13"/>
+    <hyperlink ref="F10" r:id="rId14"/>
+    <hyperlink ref="F11" r:id="rId15"/>
+    <hyperlink ref="F12" r:id="rId16"/>
+    <hyperlink ref="F13" r:id="rId17"/>
+    <hyperlink ref="I13" r:id="rId18" location="@lounge.jpg"/>
+    <hyperlink ref="W13" r:id="rId19"/>
+    <hyperlink ref="F14" r:id="rId20"/>
+    <hyperlink ref="X14" r:id="rId21"/>
+    <hyperlink ref="AA14" r:id="rId22"/>
+    <hyperlink ref="AL14" r:id="rId23"/>
+    <hyperlink ref="AN14" r:id="rId24"/>
+    <hyperlink ref="AO14" r:id="rId25"/>
+    <hyperlink ref="AP14" r:id="rId26"/>
+    <hyperlink ref="BA14" r:id="rId27"/>
+    <hyperlink ref="F15" r:id="rId28"/>
+    <hyperlink ref="X15" r:id="rId29"/>
+    <hyperlink ref="Q16" r:id="rId30" location="@lounge.jpg"/>
+    <hyperlink ref="BN16" r:id="rId31" location="@Ebay@#@23.50&amp;euro;@###@https://testing.xataka.com@#@Xataka@#@15,670&amp;euro;"/>
+    <hyperlink ref="BS16" r:id="rId32"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -9671,7 +9727,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:78" ht="15.75" customHeight="1">
       <c r="A1" s="34" t="s">
@@ -10065,36 +10121,36 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="H2" r:id="rId3" location="#@http://www.amazon.in/Forzza-Daniel-Large-Finish-Wenge/dp/B01ELJQSS8@##@http://www.amazon.in/Nubia-Z11-Mini-Gold/dp/B01N6MTTV8@##@http://www.amazon.in/Samsung-Z2-SM-Z200F-Gold-8GB/dp/B01LW4PPFV" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="J2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="K2" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="H3" r:id="rId6" location="#@http://www.amazon.in/Forzza-Daniel-Large-Finish-Wenge/dp/B01ELJQSS8@##@http://www.amazon.in/Nubia-Z11-Mini-Gold/dp/B01N6MTTV8@##@http://www.amazon.in/Samsung-Z2-SM-Z200F-Gold-8GB/dp/B01LW4PPFV" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="W3" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="H2" r:id="rId3" location="#@http://www.amazon.in/Forzza-Daniel-Large-Finish-Wenge/dp/B01ELJQSS8@##@http://www.amazon.in/Nubia-Z11-Mini-Gold/dp/B01N6MTTV8@##@http://www.amazon.in/Samsung-Z2-SM-Z200F-Gold-8GB/dp/B01LW4PPFV"/>
+    <hyperlink ref="J2" r:id="rId4"/>
+    <hyperlink ref="K2" r:id="rId5"/>
+    <hyperlink ref="H3" r:id="rId6" location="#@http://www.amazon.in/Forzza-Daniel-Large-Finish-Wenge/dp/B01ELJQSS8@##@http://www.amazon.in/Nubia-Z11-Mini-Gold/dp/B01N6MTTV8@##@http://www.amazon.in/Samsung-Z2-SM-Z200F-Gold-8GB/dp/B01LW4PPFV"/>
+    <hyperlink ref="W3" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:CH2"/>
+  <dimension ref="A1:CP2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="CA1" workbookViewId="0">
+      <selection activeCell="CK2" sqref="CK2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="85" max="85" width="27.5" customWidth="1" collapsed="1"/>
-    <col min="86" max="86" width="35.6640625" customWidth="1" collapsed="1"/>
+    <col min="85" max="85" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="86" max="86" width="35.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" ht="64">
+    <row r="1" spans="1:94" ht="63">
       <c r="A1" s="54" t="s">
         <v>16</v>
       </c>
@@ -10353,8 +10409,32 @@
       <c r="CH1" s="58" t="s">
         <v>306</v>
       </c>
+      <c r="CI1" s="132" t="s">
+        <v>585</v>
+      </c>
+      <c r="CJ1" s="132" t="s">
+        <v>586</v>
+      </c>
+      <c r="CK1" s="55" t="s">
+        <v>587</v>
+      </c>
+      <c r="CL1" s="55" t="s">
+        <v>588</v>
+      </c>
+      <c r="CM1" s="55" t="s">
+        <v>589</v>
+      </c>
+      <c r="CN1" s="55" t="s">
+        <v>590</v>
+      </c>
+      <c r="CO1" s="55" t="s">
+        <v>591</v>
+      </c>
+      <c r="CP1" s="55" t="s">
+        <v>592</v>
+      </c>
     </row>
-    <row r="2" spans="1:86" ht="15.75" customHeight="1">
+    <row r="2" spans="1:94" ht="15.75" customHeight="1">
       <c r="A2" s="60" t="s">
         <v>170</v>
       </c>
@@ -10612,58 +10692,83 @@
       </c>
       <c r="CH2" s="71" t="s">
         <v>177</v>
+      </c>
+      <c r="CI2" s="133" t="s">
+        <v>177</v>
+      </c>
+      <c r="CJ2" s="133" t="s">
+        <v>198</v>
+      </c>
+      <c r="CK2" s="134" t="s">
+        <v>593</v>
+      </c>
+      <c r="CL2" s="133" t="s">
+        <v>594</v>
+      </c>
+      <c r="CM2" s="135" t="s">
+        <v>595</v>
+      </c>
+      <c r="CN2" s="136" t="s">
+        <v>596</v>
+      </c>
+      <c r="CO2" s="134" t="s">
+        <v>598</v>
+      </c>
+      <c r="CP2" s="134" t="s">
+        <v>597</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" location="@lounge.jpg" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="BS2" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="Q2" r:id="rId1" location="@lounge.jpg"/>
+    <hyperlink ref="BS2" r:id="rId2"/>
+    <hyperlink ref="F2" r:id="rId3"/>
+    <hyperlink ref="CM2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.83203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.1640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="20" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.6640625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="16" customWidth="1" collapsed="1"/>
     <col min="13" max="14" width="18" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.5" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.1640625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="13.83203125" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.1640625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="21.33203125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="21.28515625" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="24" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="27.5" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="15.83203125" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="16.6640625" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="15.5" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="15.42578125" customWidth="1" collapsed="1"/>
     <col min="26" max="26" width="19" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="14" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.1640625" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="17.1640625" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="14.33203125" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="14.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" s="106" customFormat="1" ht="45" customHeight="1">
@@ -10900,8 +11005,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Y2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" display="https://www.youtube.com/embed/Ce7dDso0TfU" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="Y2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2" display="https://www.youtube.com/embed/Ce7dDso0TfU"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -10909,7 +11014,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -10917,7 +11022,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="51" t="s">
@@ -10969,17 +11074,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
-    <hyperlink ref="A5" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
-    <hyperlink ref="A6" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A6" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -10987,7 +11092,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1">
       <c r="A1" s="80" t="s">
@@ -11946,17 +12051,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:AB17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" customHeight="1">
       <c r="A1" s="94" t="s">

</xml_diff>

<commit_message>
LFE - fichaDeReview_lfe()- 4 files modified
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/excel.xlsx
+++ b/Aml_automation/src/Common/excel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="23040" windowHeight="12435" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="23040" windowHeight="12435" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="TagCatagory" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2615" uniqueCount="599">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2615" uniqueCount="600">
   <si>
     <t>Table Type</t>
   </si>
@@ -1825,6 +1825,9 @@
   </si>
   <si>
     <t>hookimage.jpeg</t>
+  </si>
+  <si>
+    <t>7@##@No parece importar mucho que ferias como el CES 2017 hayan sido.@##@testing worst input ficha testing ficha testing ficha.@##@diseno@###@7@~#~@automate@###@8@##@Preguntas y respuestas sobre el supuesto nuevo canon digital: ¿quién tendrá que pagarlo y por qué?</t>
   </si>
 </sst>
 </file>
@@ -2881,7 +2884,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2916,6 +2918,21 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2940,20 +2957,8 @@
     <xf numFmtId="0" fontId="14" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5311,42 +5316,42 @@
       <c r="C1" s="95" t="s">
         <v>514</v>
       </c>
-      <c r="D1" s="126" t="s">
+      <c r="D1" s="130" t="s">
         <v>518</v>
       </c>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
       <c r="G1" s="96"/>
-      <c r="H1" s="128" t="s">
+      <c r="H1" s="132" t="s">
         <v>522</v>
       </c>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
-      <c r="K1" s="129"/>
-      <c r="L1" s="130" t="s">
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="133"/>
+      <c r="L1" s="134" t="s">
         <v>526</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="123" t="s">
+      <c r="M1" s="128"/>
+      <c r="N1" s="128"/>
+      <c r="O1" s="129"/>
+      <c r="P1" s="127" t="s">
         <v>530</v>
       </c>
-      <c r="Q1" s="124"/>
-      <c r="R1" s="124"/>
-      <c r="S1" s="125"/>
-      <c r="T1" s="131" t="s">
+      <c r="Q1" s="128"/>
+      <c r="R1" s="128"/>
+      <c r="S1" s="129"/>
+      <c r="T1" s="135" t="s">
         <v>533</v>
       </c>
-      <c r="U1" s="124"/>
-      <c r="V1" s="124"/>
-      <c r="W1" s="125"/>
-      <c r="X1" s="123" t="s">
+      <c r="U1" s="128"/>
+      <c r="V1" s="128"/>
+      <c r="W1" s="129"/>
+      <c r="X1" s="127" t="s">
         <v>535</v>
       </c>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="125"/>
+      <c r="Y1" s="128"/>
+      <c r="Z1" s="128"/>
+      <c r="AA1" s="129"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1">
       <c r="A2" s="94" t="s">
@@ -10140,7 +10145,7 @@
   </sheetPr>
   <dimension ref="A1:CP2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CA1" workbookViewId="0">
+    <sheetView topLeftCell="CA1" workbookViewId="0">
       <selection activeCell="CK2" sqref="CK2"/>
     </sheetView>
   </sheetViews>
@@ -10409,10 +10414,10 @@
       <c r="CH1" s="58" t="s">
         <v>306</v>
       </c>
-      <c r="CI1" s="132" t="s">
+      <c r="CI1" s="119" t="s">
         <v>585</v>
       </c>
-      <c r="CJ1" s="132" t="s">
+      <c r="CJ1" s="119" t="s">
         <v>586</v>
       </c>
       <c r="CK1" s="55" t="s">
@@ -10693,28 +10698,28 @@
       <c r="CH2" s="71" t="s">
         <v>177</v>
       </c>
-      <c r="CI2" s="133" t="s">
-        <v>177</v>
-      </c>
-      <c r="CJ2" s="133" t="s">
-        <v>198</v>
-      </c>
-      <c r="CK2" s="134" t="s">
+      <c r="CI2" s="120" t="s">
+        <v>177</v>
+      </c>
+      <c r="CJ2" s="120" t="s">
+        <v>198</v>
+      </c>
+      <c r="CK2" s="121" t="s">
         <v>593</v>
       </c>
-      <c r="CL2" s="133" t="s">
+      <c r="CL2" s="120" t="s">
         <v>594</v>
       </c>
-      <c r="CM2" s="135" t="s">
+      <c r="CM2" s="122" t="s">
         <v>595</v>
       </c>
-      <c r="CN2" s="136" t="s">
+      <c r="CN2" s="123" t="s">
         <v>596</v>
       </c>
-      <c r="CO2" s="134" t="s">
+      <c r="CO2" s="121" t="s">
         <v>598</v>
       </c>
-      <c r="CP2" s="134" t="s">
+      <c r="CP2" s="121" t="s">
         <v>597</v>
       </c>
     </row>
@@ -10733,8 +10738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -10906,17 +10911,17 @@
       <c r="F2" s="63" t="s">
         <v>177</v>
       </c>
-      <c r="G2" s="108" t="s">
+      <c r="G2" s="107" t="s">
         <v>584</v>
       </c>
       <c r="H2" s="65" t="s">
         <v>583</v>
       </c>
-      <c r="I2" s="107" t="s">
+      <c r="I2" s="136" t="s">
         <v>581</v>
       </c>
       <c r="J2" s="63" t="s">
-        <v>177</v>
+        <v>599</v>
       </c>
       <c r="K2" s="63" t="s">
         <v>177</v>
@@ -11104,13 +11109,13 @@
       <c r="C1" s="81" t="s">
         <v>407</v>
       </c>
-      <c r="D1" s="120" t="s">
+      <c r="D1" s="124" t="s">
         <v>413</v>
       </c>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="122"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="125"/>
+      <c r="H1" s="126"/>
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
       <c r="K1" s="25"/>
@@ -12076,42 +12081,42 @@
       <c r="D1" s="95" t="s">
         <v>514</v>
       </c>
-      <c r="E1" s="126" t="s">
+      <c r="E1" s="130" t="s">
         <v>518</v>
       </c>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
       <c r="H1" s="96"/>
-      <c r="I1" s="128" t="s">
+      <c r="I1" s="132" t="s">
         <v>522</v>
       </c>
-      <c r="J1" s="127"/>
-      <c r="K1" s="127"/>
-      <c r="L1" s="129"/>
-      <c r="M1" s="130" t="s">
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
+      <c r="L1" s="133"/>
+      <c r="M1" s="134" t="s">
         <v>526</v>
       </c>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="123" t="s">
+      <c r="N1" s="128"/>
+      <c r="O1" s="128"/>
+      <c r="P1" s="129"/>
+      <c r="Q1" s="127" t="s">
         <v>530</v>
       </c>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="125"/>
-      <c r="U1" s="131" t="s">
+      <c r="R1" s="128"/>
+      <c r="S1" s="128"/>
+      <c r="T1" s="129"/>
+      <c r="U1" s="135" t="s">
         <v>533</v>
       </c>
-      <c r="V1" s="124"/>
-      <c r="W1" s="124"/>
-      <c r="X1" s="125"/>
-      <c r="Y1" s="123" t="s">
+      <c r="V1" s="128"/>
+      <c r="W1" s="128"/>
+      <c r="X1" s="129"/>
+      <c r="Y1" s="127" t="s">
         <v>535</v>
       </c>
-      <c r="Z1" s="124"/>
-      <c r="AA1" s="124"/>
-      <c r="AB1" s="125"/>
+      <c r="Z1" s="128"/>
+      <c r="AA1" s="128"/>
+      <c r="AB1" s="129"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="94" t="s">
@@ -12200,1290 +12205,1290 @@
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A3" s="109" t="s">
+      <c r="A3" s="108" t="s">
         <v>560</v>
       </c>
-      <c r="B3" s="109" t="s">
+      <c r="B3" s="108" t="s">
         <v>561</v>
       </c>
-      <c r="C3" s="109" t="s">
+      <c r="C3" s="108" t="s">
         <v>562</v>
       </c>
-      <c r="D3" s="110" t="s">
+      <c r="D3" s="109" t="s">
         <v>167</v>
       </c>
-      <c r="E3" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="F3" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="G3" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="H3" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="I3" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="J3" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="K3" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="L3" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="M3" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="N3" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="O3" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="P3" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q3" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="R3" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="S3" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="T3" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="U3" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="V3" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="W3" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="X3" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y3" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z3" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA3" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB3" s="112" t="s">
+      <c r="E3" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="F3" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="G3" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="H3" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="I3" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="J3" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="K3" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="L3" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="M3" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="N3" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="O3" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="P3" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q3" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="R3" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="S3" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="T3" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="U3" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="V3" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="W3" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="X3" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y3" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z3" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA3" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB3" s="111" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A4" s="109" t="s">
+      <c r="A4" s="108" t="s">
         <v>560</v>
       </c>
-      <c r="B4" s="109" t="s">
+      <c r="B4" s="108" t="s">
         <v>561</v>
       </c>
-      <c r="C4" s="109" t="s">
+      <c r="C4" s="108" t="s">
         <v>563</v>
       </c>
-      <c r="D4" s="110" t="s">
+      <c r="D4" s="109" t="s">
         <v>564</v>
       </c>
-      <c r="E4" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="F4" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="G4" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="H4" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="I4" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="J4" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="K4" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="L4" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="M4" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="N4" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="O4" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="P4" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q4" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="R4" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="S4" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="T4" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="U4" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="V4" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="W4" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="X4" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y4" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z4" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA4" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB4" s="112" t="s">
+      <c r="E4" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="G4" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="H4" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="I4" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="J4" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="K4" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="L4" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="M4" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="N4" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="O4" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="P4" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q4" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="R4" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="S4" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="T4" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="U4" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="V4" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="W4" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="X4" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y4" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z4" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA4" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB4" s="111" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A5" s="109" t="s">
+      <c r="A5" s="108" t="s">
         <v>560</v>
       </c>
-      <c r="B5" s="109" t="s">
+      <c r="B5" s="108" t="s">
         <v>561</v>
       </c>
-      <c r="C5" s="109" t="s">
+      <c r="C5" s="108" t="s">
         <v>565</v>
       </c>
-      <c r="D5" s="110" t="s">
+      <c r="D5" s="109" t="s">
         <v>566</v>
       </c>
-      <c r="E5" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="F5" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="G5" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="H5" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="I5" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="J5" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="K5" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="L5" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="M5" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="N5" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="O5" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="P5" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q5" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="R5" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="S5" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="T5" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="U5" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="V5" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="W5" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="X5" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y5" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z5" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA5" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="AB5" s="112" t="s">
+      <c r="E5" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="F5" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="G5" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="H5" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="I5" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="J5" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="K5" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="L5" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="M5" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="N5" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="O5" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="P5" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q5" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="R5" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="S5" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="T5" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="U5" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="V5" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="W5" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="X5" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y5" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z5" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA5" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB5" s="111" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="108" t="s">
         <v>560</v>
       </c>
-      <c r="B6" s="109" t="s">
+      <c r="B6" s="108" t="s">
         <v>561</v>
       </c>
-      <c r="C6" s="109" t="s">
+      <c r="C6" s="108" t="s">
         <v>567</v>
       </c>
-      <c r="D6" s="110" t="s">
+      <c r="D6" s="109" t="s">
         <v>568</v>
       </c>
-      <c r="E6" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="F6" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="G6" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="H6" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="I6" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="J6" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="K6" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="L6" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="M6" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="N6" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="O6" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="P6" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q6" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="R6" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="S6" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="T6" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="U6" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="V6" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="W6" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="X6" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="Y6" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z6" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA6" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB6" s="112" t="s">
+      <c r="E6" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="F6" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="G6" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="H6" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="I6" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="J6" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="K6" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="L6" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="M6" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="N6" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="O6" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="P6" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q6" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="R6" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="S6" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="T6" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="U6" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="V6" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="W6" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="X6" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y6" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z6" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA6" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB6" s="111" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A7" s="109" t="s">
+      <c r="A7" s="108" t="s">
         <v>569</v>
       </c>
-      <c r="B7" s="109" t="s">
+      <c r="B7" s="108" t="s">
         <v>561</v>
       </c>
-      <c r="C7" s="109" t="s">
+      <c r="C7" s="108" t="s">
         <v>567</v>
       </c>
-      <c r="D7" s="110" t="s">
+      <c r="D7" s="109" t="s">
         <v>570</v>
       </c>
-      <c r="E7" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="F7" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="G7" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="H7" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="I7" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="J7" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="K7" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="L7" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="M7" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="N7" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="O7" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="P7" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q7" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="R7" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="S7" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="T7" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="U7" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="V7" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="W7" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="X7" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y7" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z7" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA7" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB7" s="112" t="s">
+      <c r="E7" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="F7" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="G7" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="H7" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="I7" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="J7" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="K7" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="L7" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="M7" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="N7" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="O7" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="P7" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q7" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="R7" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="S7" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="T7" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="U7" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="V7" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="W7" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="X7" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y7" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z7" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA7" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB7" s="111" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A8" s="109" t="s">
+      <c r="A8" s="108" t="s">
         <v>571</v>
       </c>
-      <c r="B8" s="109" t="s">
+      <c r="B8" s="108" t="s">
         <v>169</v>
       </c>
-      <c r="C8" s="109" t="s">
+      <c r="C8" s="108" t="s">
         <v>562</v>
       </c>
-      <c r="D8" s="110" t="s">
+      <c r="D8" s="109" t="s">
         <v>167</v>
       </c>
-      <c r="E8" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="F8" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="G8" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="H8" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="I8" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="J8" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="K8" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="L8" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="M8" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="N8" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="O8" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="P8" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q8" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="R8" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="S8" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="T8" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="U8" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="V8" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="W8" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="X8" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y8" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z8" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA8" s="114"/>
-      <c r="AB8" s="112" t="s">
+      <c r="E8" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="G8" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="H8" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="I8" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="J8" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="K8" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="L8" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="M8" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="N8" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="O8" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="P8" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q8" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="R8" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="S8" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="T8" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="U8" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="V8" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="W8" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="X8" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y8" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z8" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA8" s="113"/>
+      <c r="AB8" s="111" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A9" s="115" t="s">
+      <c r="A9" s="114" t="s">
         <v>571</v>
       </c>
-      <c r="B9" s="115" t="s">
+      <c r="B9" s="114" t="s">
         <v>169</v>
       </c>
-      <c r="C9" s="115" t="s">
+      <c r="C9" s="114" t="s">
         <v>563</v>
       </c>
-      <c r="D9" s="116" t="s">
+      <c r="D9" s="115" t="s">
         <v>564</v>
       </c>
-      <c r="E9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="F9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="G9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="H9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="I9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="J9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="K9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="L9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="M9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="N9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="O9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="P9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="R9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="S9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="T9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="U9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="V9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="W9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="X9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="Y9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA9" s="118" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB9" s="117" t="s">
+      <c r="E9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="F9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="G9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="H9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="I9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="J9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="K9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="L9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="M9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="N9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="O9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="P9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="R9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="S9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="T9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="U9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="V9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="W9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="X9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z9" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA9" s="117" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB9" s="116" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A10" s="109" t="s">
+      <c r="A10" s="108" t="s">
         <v>571</v>
       </c>
-      <c r="B10" s="109" t="s">
+      <c r="B10" s="108" t="s">
         <v>169</v>
       </c>
-      <c r="C10" s="109" t="s">
+      <c r="C10" s="108" t="s">
         <v>567</v>
       </c>
-      <c r="D10" s="110" t="s">
+      <c r="D10" s="109" t="s">
         <v>572</v>
       </c>
-      <c r="E10" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="F10" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="G10" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="H10" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="I10" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="J10" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="K10" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="L10" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="M10" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="N10" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="O10" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="P10" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q10" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="R10" s="119" t="s">
-        <v>179</v>
-      </c>
-      <c r="S10" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="T10" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="U10" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="V10" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="W10" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="X10" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y10" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z10" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA10" s="119" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB10" s="112" t="s">
+      <c r="E10" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="G10" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="H10" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="I10" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="J10" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="K10" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="L10" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="M10" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="N10" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="O10" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="P10" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q10" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="R10" s="118" t="s">
+        <v>179</v>
+      </c>
+      <c r="S10" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="T10" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="U10" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="V10" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="W10" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="X10" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y10" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z10" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA10" s="118" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB10" s="111" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A11" s="109" t="s">
+      <c r="A11" s="108" t="s">
         <v>571</v>
       </c>
-      <c r="B11" s="109" t="s">
+      <c r="B11" s="108" t="s">
         <v>169</v>
       </c>
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="108" t="s">
         <v>565</v>
       </c>
-      <c r="D11" s="110" t="s">
+      <c r="D11" s="109" t="s">
         <v>566</v>
       </c>
-      <c r="E11" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="F11" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="G11" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="H11" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="I11" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="J11" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="K11" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="L11" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="M11" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="N11" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="O11" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="P11" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q11" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="R11" s="119" t="s">
-        <v>179</v>
-      </c>
-      <c r="S11" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="T11" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="U11" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="V11" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="W11" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="X11" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y11" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z11" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA11" s="119" t="s">
-        <v>198</v>
-      </c>
-      <c r="AB11" s="112" t="s">
+      <c r="E11" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="F11" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="G11" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="H11" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="I11" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="J11" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="K11" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="L11" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="M11" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="N11" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="O11" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="P11" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q11" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="R11" s="118" t="s">
+        <v>179</v>
+      </c>
+      <c r="S11" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="T11" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="U11" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="V11" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="W11" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="X11" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y11" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z11" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA11" s="118" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB11" s="111" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A12" s="109" t="s">
+      <c r="A12" s="108" t="s">
         <v>573</v>
       </c>
-      <c r="B12" s="109" t="s">
+      <c r="B12" s="108" t="s">
         <v>167</v>
       </c>
-      <c r="C12" s="109" t="s">
+      <c r="C12" s="108" t="s">
         <v>565</v>
       </c>
-      <c r="D12" s="110" t="s">
+      <c r="D12" s="109" t="s">
         <v>566</v>
       </c>
-      <c r="E12" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="F12" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="G12" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="H12" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="I12" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="J12" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="K12" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="L12" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="M12" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="N12" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="O12" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="P12" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q12" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="R12" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="S12" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="T12" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="U12" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="V12" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="W12" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="X12" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y12" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z12" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA12" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB12" s="112" t="s">
+      <c r="E12" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="G12" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="H12" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="I12" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="J12" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="K12" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="L12" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="M12" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="N12" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="O12" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="P12" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q12" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="R12" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="S12" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="T12" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="U12" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="V12" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="W12" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="X12" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y12" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z12" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA12" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB12" s="111" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A13" s="109" t="s">
+      <c r="A13" s="108" t="s">
         <v>573</v>
       </c>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="108" t="s">
         <v>167</v>
       </c>
-      <c r="C13" s="109" t="s">
+      <c r="C13" s="108" t="s">
         <v>567</v>
       </c>
-      <c r="D13" s="110" t="s">
+      <c r="D13" s="109" t="s">
         <v>570</v>
       </c>
-      <c r="E13" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="F13" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="G13" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="H13" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="I13" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="J13" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="K13" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="L13" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="M13" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="N13" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="O13" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="P13" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q13" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="R13" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="S13" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="T13" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="U13" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="V13" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="W13" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="X13" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y13" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z13" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA13" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB13" s="112" t="s">
+      <c r="E13" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="F13" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="G13" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="H13" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="I13" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="J13" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="K13" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="L13" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="M13" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="N13" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="O13" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="P13" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q13" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="R13" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="S13" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="T13" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="U13" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="V13" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="W13" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="X13" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y13" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z13" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA13" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB13" s="111" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A14" s="109" t="s">
+      <c r="A14" s="108" t="s">
         <v>170</v>
       </c>
-      <c r="B14" s="109" t="s">
+      <c r="B14" s="108" t="s">
         <v>170</v>
       </c>
-      <c r="C14" s="109" t="s">
+      <c r="C14" s="108" t="s">
         <v>562</v>
       </c>
-      <c r="D14" s="110" t="s">
+      <c r="D14" s="109" t="s">
         <v>167</v>
       </c>
-      <c r="E14" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="F14" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="G14" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="H14" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="I14" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="J14" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="K14" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="L14" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="M14" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="N14" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="O14" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="P14" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q14" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="R14" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="S14" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="T14" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="U14" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="V14" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="W14" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="X14" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y14" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z14" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA14" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB14" s="112" t="s">
+      <c r="E14" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="F14" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="G14" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="H14" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="I14" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="J14" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="K14" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="L14" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="M14" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="N14" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="O14" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="P14" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q14" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="R14" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="S14" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="T14" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="U14" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="V14" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="W14" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="X14" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y14" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z14" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA14" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB14" s="111" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A15" s="109" t="s">
+      <c r="A15" s="108" t="s">
         <v>170</v>
       </c>
-      <c r="B15" s="109" t="s">
+      <c r="B15" s="108" t="s">
         <v>170</v>
       </c>
-      <c r="C15" s="109" t="s">
+      <c r="C15" s="108" t="s">
         <v>563</v>
       </c>
-      <c r="D15" s="110" t="s">
+      <c r="D15" s="109" t="s">
         <v>574</v>
       </c>
-      <c r="E15" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="F15" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="G15" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="H15" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="I15" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="J15" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="K15" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="L15" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="M15" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="N15" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="O15" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="P15" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q15" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="R15" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="S15" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="T15" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="U15" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="V15" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="W15" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="X15" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y15" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z15" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA15" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB15" s="112" t="s">
+      <c r="E15" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="F15" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="G15" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="H15" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="I15" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="J15" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="K15" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="L15" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="M15" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="N15" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="O15" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="P15" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q15" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="R15" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="S15" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="T15" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="U15" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="V15" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="W15" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="X15" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y15" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z15" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA15" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB15" s="111" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A16" s="109" t="s">
+      <c r="A16" s="108" t="s">
         <v>170</v>
       </c>
-      <c r="B16" s="109" t="s">
+      <c r="B16" s="108" t="s">
         <v>170</v>
       </c>
-      <c r="C16" s="109" t="s">
+      <c r="C16" s="108" t="s">
         <v>565</v>
       </c>
-      <c r="D16" s="110" t="s">
+      <c r="D16" s="109" t="s">
         <v>566</v>
       </c>
-      <c r="E16" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="F16" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="G16" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="H16" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="I16" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="J16" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="K16" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="L16" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="M16" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="N16" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="O16" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="P16" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q16" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="R16" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="S16" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="T16" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="U16" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="V16" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="W16" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="X16" s="113" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y16" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z16" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA16" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="AB16" s="112" t="s">
+      <c r="E16" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="F16" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="G16" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="H16" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="I16" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="J16" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="K16" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="L16" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="M16" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="N16" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="O16" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="P16" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q16" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="R16" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="S16" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="T16" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="U16" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="V16" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="W16" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="X16" s="112" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y16" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z16" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA16" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB16" s="111" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A17" s="109" t="s">
+      <c r="A17" s="108" t="s">
         <v>170</v>
       </c>
-      <c r="B17" s="109" t="s">
+      <c r="B17" s="108" t="s">
         <v>170</v>
       </c>
-      <c r="C17" s="109" t="s">
+      <c r="C17" s="108" t="s">
         <v>575</v>
       </c>
-      <c r="D17" s="110" t="s">
+      <c r="D17" s="109" t="s">
         <v>568</v>
       </c>
-      <c r="E17" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="F17" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="G17" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="H17" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="I17" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="J17" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="K17" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="L17" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="M17" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="N17" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="O17" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="P17" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q17" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="R17" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="S17" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="T17" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="U17" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="V17" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="W17" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="X17" s="113" t="s">
-        <v>179</v>
-      </c>
-      <c r="Y17" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z17" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA17" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB17" s="112" t="s">
+      <c r="E17" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="F17" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="G17" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="H17" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="I17" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="J17" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="K17" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="L17" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="M17" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="N17" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="O17" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="P17" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q17" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="R17" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="S17" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="T17" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="U17" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="V17" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="W17" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="X17" s="112" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y17" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z17" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA17" s="111" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB17" s="111" t="s">
         <v>179</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1. Updated CreateMVPPostExcel class file.
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/excel.xlsx
+++ b/Aml_automation/src/Common/excel.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AML-1\git\Automation\Aml_automation\src\Common\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isha/git/Automation/Aml_automation/src/Common/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8F02FBD5-B531-974D-AC37-801D930BCBF4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="23040" windowHeight="12435" firstSheet="4" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="12440" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TagCatagory" sheetId="1" r:id="rId1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2615" uniqueCount="600">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2719" uniqueCount="619">
   <si>
     <t>Table Type</t>
   </si>
@@ -1767,24 +1768,6 @@
     <t>https://www.youtube.com/embed/azxoVRTwlNg</t>
   </si>
   <si>
-    <t>Longform</t>
-  </si>
-  <si>
-    <t>Longform post automation testing</t>
-  </si>
-  <si>
-    <t>Ficha_tecnica_title@@#@@Version2.21@@#@@https://i.blogs.es/9a59f8/samsung-nand/650_1200.jpg@@#@@https://i.blogs.es/9c2494/mi-mix/650_1200.jpg@@#@@Text11@#@Some text11@#@https://www.gmail.com@&amp;@Text22@#@Some text22@#@https://yahoo.com@&amp;@Text33@#@Some text33@#@www.google.com@&amp;@Text44@#@Some Text44@#@https://www.yahoo.com@&amp;@Text55@#@Some text55@#@http://www.outlook.com@@#@@Other details</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>fullscreen</t>
-  </si>
-  <si>
-    <t>En ella encontrarás detalles, ideas y gadgets a partir de 10 euros.</t>
-  </si>
-  <si>
     <t>Publish_to_homepage_checkbox</t>
   </si>
   <si>
@@ -1827,14 +1810,89 @@
     <t>hookimage.jpeg</t>
   </si>
   <si>
-    <t>7@##@No parece importar mucho que ferias como el CES 2017 hayan sido.@##@testing worst input ficha testing ficha testing ficha.@##@diseno@###@7@~#~@automate@###@8@##@Preguntas y respuestas sobre el supuesto nuevo canon digital: ¿quién tendrá que pagarlo y por qué?</t>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>imageLayout</t>
+  </si>
+  <si>
+    <t>video_layout</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>rich_alternativo</t>
+  </si>
+  <si>
+    <t>rich_text</t>
+  </si>
+  <si>
+    <t>rich_url</t>
+  </si>
+  <si>
+    <t>Disclaimer</t>
+  </si>
+  <si>
+    <t>Contenido_Patrocinado</t>
+  </si>
+  <si>
+    <t>brand alfa</t>
+  </si>
+  <si>
+    <t>Isha alfa</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=p6LcnmsVhc0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=kj1HCbm6fp4</t>
+  </si>
+  <si>
+    <t>Testng</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/p/BWxoQQGIJQW</t>
+  </si>
+  <si>
+    <t>https://infogr.am/be7b47aa-3d58-44da-a246-c015889c0459</t>
+  </si>
+  <si>
+    <t>grande</t>
+  </si>
+  <si>
+    <t>vidaextra</t>
+  </si>
+  <si>
+    <t>https://testing.xataka.com/seleccion/isha-normal-post-1</t>
+  </si>
+  <si>
+    <t>imagen alternativa</t>
+  </si>
+  <si>
+    <t>testing testing</t>
+  </si>
+  <si>
+    <t>https://i.blogs.es/de2d90/steam-link/1366_2000.jpg</t>
+  </si>
+  <si>
+    <t>Espacio Alcatel</t>
+  </si>
+  <si>
+    <t>Nokia</t>
+  </si>
+  <si>
+    <t>https://twitter.com/marcvidal/status/963332880972775424</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="37">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="39">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2064,16 +2122,29 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="21"/>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0066CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF333333"/>
-      <name val="Charter"/>
-      <family val="1"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="15">
@@ -2568,7 +2639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2878,13 +2949,9 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2957,9 +3024,13 @@
     <xf numFmtId="0" fontId="14" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3240,7 +3311,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -3248,7 +3319,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:1024" ht="15.75" customHeight="1">
       <c r="A1" s="5" t="s">
@@ -4296,7 +4367,7 @@
       <c r="AMI1" s="25"/>
       <c r="AMJ1" s="25"/>
     </row>
-    <row r="2" spans="1:1024">
+    <row r="2" spans="1:1024" ht="16">
       <c r="A2" s="9" t="s">
         <v>240</v>
       </c>
@@ -4326,7 +4397,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="1:1024">
+    <row r="3" spans="1:1024" ht="16">
       <c r="A3" s="9" t="s">
         <v>263</v>
       </c>
@@ -4360,7 +4431,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:1024">
+    <row r="4" spans="1:1024" ht="16">
       <c r="A4" s="9" t="s">
         <v>277</v>
       </c>
@@ -4392,7 +4463,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="1:1024">
+    <row r="5" spans="1:1024" ht="16">
       <c r="A5" s="9" t="s">
         <v>286</v>
       </c>
@@ -4420,7 +4491,7 @@
       </c>
       <c r="L5" s="18"/>
     </row>
-    <row r="6" spans="1:1024">
+    <row r="6" spans="1:1024" ht="16">
       <c r="A6" s="9" t="s">
         <v>299</v>
       </c>
@@ -5242,7 +5313,7 @@
       <c r="K38" s="25"/>
       <c r="L38" s="25"/>
     </row>
-    <row r="39" spans="1:12" ht="12.75">
+    <row r="39" spans="1:12" ht="14">
       <c r="A39" s="9" t="s">
         <v>527</v>
       </c>
@@ -5266,7 +5337,7 @@
       <c r="K39" s="25"/>
       <c r="L39" s="25"/>
     </row>
-    <row r="40" spans="1:12" ht="12.75">
+    <row r="40" spans="1:12" ht="14">
       <c r="A40" s="20" t="s">
         <v>531</v>
       </c>
@@ -5296,7 +5367,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -5304,7 +5375,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1" s="94" t="s">
@@ -5316,42 +5387,42 @@
       <c r="C1" s="95" t="s">
         <v>514</v>
       </c>
-      <c r="D1" s="130" t="s">
+      <c r="D1" s="128" t="s">
         <v>518</v>
       </c>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
+      <c r="E1" s="129"/>
+      <c r="F1" s="129"/>
       <c r="G1" s="96"/>
-      <c r="H1" s="132" t="s">
+      <c r="H1" s="130" t="s">
         <v>522</v>
       </c>
-      <c r="I1" s="131"/>
-      <c r="J1" s="131"/>
-      <c r="K1" s="133"/>
-      <c r="L1" s="134" t="s">
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="131"/>
+      <c r="L1" s="132" t="s">
         <v>526</v>
       </c>
-      <c r="M1" s="128"/>
-      <c r="N1" s="128"/>
-      <c r="O1" s="129"/>
-      <c r="P1" s="127" t="s">
+      <c r="M1" s="126"/>
+      <c r="N1" s="126"/>
+      <c r="O1" s="127"/>
+      <c r="P1" s="125" t="s">
         <v>530</v>
       </c>
-      <c r="Q1" s="128"/>
-      <c r="R1" s="128"/>
-      <c r="S1" s="129"/>
-      <c r="T1" s="135" t="s">
+      <c r="Q1" s="126"/>
+      <c r="R1" s="126"/>
+      <c r="S1" s="127"/>
+      <c r="T1" s="133" t="s">
         <v>533</v>
       </c>
-      <c r="U1" s="128"/>
-      <c r="V1" s="128"/>
-      <c r="W1" s="129"/>
-      <c r="X1" s="127" t="s">
+      <c r="U1" s="126"/>
+      <c r="V1" s="126"/>
+      <c r="W1" s="127"/>
+      <c r="X1" s="125" t="s">
         <v>535</v>
       </c>
-      <c r="Y1" s="128"/>
-      <c r="Z1" s="128"/>
-      <c r="AA1" s="129"/>
+      <c r="Y1" s="126"/>
+      <c r="Z1" s="126"/>
+      <c r="AA1" s="127"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1">
       <c r="A2" s="94" t="s">
@@ -5450,7 +5521,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -5458,7 +5529,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -5748,51 +5819,51 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="E2" r:id="rId3"/>
-    <hyperlink ref="F2" r:id="rId4"/>
-    <hyperlink ref="J2" r:id="rId5"/>
-    <hyperlink ref="K2" r:id="rId6"/>
-    <hyperlink ref="L2" r:id="rId7"/>
-    <hyperlink ref="B3" r:id="rId8"/>
-    <hyperlink ref="C3" r:id="rId9"/>
-    <hyperlink ref="D3" r:id="rId10"/>
-    <hyperlink ref="F3" r:id="rId11"/>
-    <hyperlink ref="J3" r:id="rId12"/>
-    <hyperlink ref="K3" r:id="rId13"/>
-    <hyperlink ref="L3" r:id="rId14"/>
-    <hyperlink ref="C4" r:id="rId15"/>
-    <hyperlink ref="D4" r:id="rId16"/>
-    <hyperlink ref="F4" r:id="rId17"/>
-    <hyperlink ref="J4" r:id="rId18"/>
-    <hyperlink ref="K4" r:id="rId19"/>
-    <hyperlink ref="L4" r:id="rId20"/>
-    <hyperlink ref="C5" r:id="rId21"/>
-    <hyperlink ref="D5" r:id="rId22"/>
-    <hyperlink ref="F5" r:id="rId23"/>
-    <hyperlink ref="J5" r:id="rId24"/>
-    <hyperlink ref="K5" r:id="rId25"/>
-    <hyperlink ref="L5" r:id="rId26"/>
-    <hyperlink ref="C6" r:id="rId27"/>
-    <hyperlink ref="D6" r:id="rId28"/>
-    <hyperlink ref="F6" r:id="rId29"/>
-    <hyperlink ref="J6" r:id="rId30"/>
-    <hyperlink ref="K6" r:id="rId31"/>
-    <hyperlink ref="L6" r:id="rId32"/>
-    <hyperlink ref="C7" r:id="rId33"/>
-    <hyperlink ref="D7" r:id="rId34"/>
-    <hyperlink ref="F7" r:id="rId35"/>
-    <hyperlink ref="J7" r:id="rId36"/>
-    <hyperlink ref="K7" r:id="rId37"/>
-    <hyperlink ref="L7" r:id="rId38"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="F2" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="J2" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="K2" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="L2" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="B3" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="C3" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="D3" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="F3" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="J3" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="K3" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="L3" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="C4" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="D4" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="F4" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="J4" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="K4" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="L4" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="C5" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="D5" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="F5" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="J5" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="K5" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="L5" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="C6" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="D6" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="F6" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="J6" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="K6" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="L6" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="C7" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="D7" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="F7" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="J7" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="K7" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="L7" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -5800,9 +5871,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:84" ht="12.75">
+    <row r="1" spans="1:84" ht="14">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -6044,7 +6115,7 @@
       <c r="CE1" s="32"/>
       <c r="CF1" s="32"/>
     </row>
-    <row r="2" spans="1:84" ht="12.75">
+    <row r="2" spans="1:84" ht="14">
       <c r="A2" s="33" t="s">
         <v>170</v>
       </c>
@@ -6286,7 +6357,7 @@
       <c r="CE2" s="36"/>
       <c r="CF2" s="36"/>
     </row>
-    <row r="3" spans="1:84" ht="12.75">
+    <row r="3" spans="1:84" ht="14">
       <c r="A3" s="33" t="s">
         <v>2</v>
       </c>
@@ -6768,7 +6839,7 @@
       <c r="CE4" s="36"/>
       <c r="CF4" s="36"/>
     </row>
-    <row r="5" spans="1:84" ht="12.75">
+    <row r="5" spans="1:84" ht="14">
       <c r="A5" s="33" t="s">
         <v>235</v>
       </c>
@@ -7010,7 +7081,7 @@
       <c r="CE5" s="36"/>
       <c r="CF5" s="36"/>
     </row>
-    <row r="6" spans="1:84" ht="12.75">
+    <row r="6" spans="1:84" ht="14">
       <c r="A6" s="41" t="s">
         <v>242</v>
       </c>
@@ -7252,7 +7323,7 @@
       <c r="CE6" s="36"/>
       <c r="CF6" s="36"/>
     </row>
-    <row r="7" spans="1:84" ht="12.75">
+    <row r="7" spans="1:84" ht="14">
       <c r="A7" s="41" t="s">
         <v>250</v>
       </c>
@@ -7494,7 +7565,7 @@
       <c r="CE7" s="36"/>
       <c r="CF7" s="36"/>
     </row>
-    <row r="8" spans="1:84" ht="12.75">
+    <row r="8" spans="1:84" ht="14">
       <c r="A8" s="36" t="s">
         <v>258</v>
       </c>
@@ -7736,7 +7807,7 @@
       <c r="CE8" s="36"/>
       <c r="CF8" s="36"/>
     </row>
-    <row r="9" spans="1:84" ht="12.75">
+    <row r="9" spans="1:84" ht="14">
       <c r="A9" s="36" t="s">
         <v>273</v>
       </c>
@@ -7978,7 +8049,7 @@
       <c r="CE9" s="36"/>
       <c r="CF9" s="36"/>
     </row>
-    <row r="10" spans="1:84" ht="12.75">
+    <row r="10" spans="1:84" ht="14">
       <c r="A10" s="36" t="s">
         <v>284</v>
       </c>
@@ -8220,7 +8291,7 @@
       <c r="CE10" s="36"/>
       <c r="CF10" s="36"/>
     </row>
-    <row r="11" spans="1:84" ht="12.75">
+    <row r="11" spans="1:84" ht="14">
       <c r="A11" s="36" t="s">
         <v>291</v>
       </c>
@@ -8462,7 +8533,7 @@
       <c r="CE11" s="36"/>
       <c r="CF11" s="36"/>
     </row>
-    <row r="12" spans="1:84" ht="12.75">
+    <row r="12" spans="1:84" ht="14">
       <c r="A12" s="36" t="s">
         <v>309</v>
       </c>
@@ -8704,7 +8775,7 @@
       <c r="CE12" s="36"/>
       <c r="CF12" s="36"/>
     </row>
-    <row r="13" spans="1:84" ht="12.75">
+    <row r="13" spans="1:84" ht="14">
       <c r="A13" s="33" t="s">
         <v>316</v>
       </c>
@@ -8946,7 +9017,7 @@
       <c r="CE13" s="36"/>
       <c r="CF13" s="36"/>
     </row>
-    <row r="14" spans="1:84" ht="12.75">
+    <row r="14" spans="1:84" ht="14">
       <c r="A14" s="36" t="s">
         <v>329</v>
       </c>
@@ -9188,7 +9259,7 @@
       <c r="CE14" s="36"/>
       <c r="CF14" s="36"/>
     </row>
-    <row r="15" spans="1:84" ht="12.75">
+    <row r="15" spans="1:84" ht="14">
       <c r="A15" s="33" t="s">
         <v>352</v>
       </c>
@@ -9430,7 +9501,7 @@
       <c r="CE15" s="36"/>
       <c r="CF15" s="36"/>
     </row>
-    <row r="16" spans="1:84" ht="15">
+    <row r="16" spans="1:84" ht="16">
       <c r="A16" s="60" t="s">
         <v>170</v>
       </c>
@@ -9686,45 +9757,45 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="I2" r:id="rId2" location="@lounge.jpg"/>
-    <hyperlink ref="O2" r:id="rId3"/>
-    <hyperlink ref="Q2" r:id="rId4"/>
-    <hyperlink ref="X2" r:id="rId5"/>
-    <hyperlink ref="AB2" r:id="rId6"/>
-    <hyperlink ref="F3" r:id="rId7"/>
-    <hyperlink ref="X3" r:id="rId8"/>
-    <hyperlink ref="F4" r:id="rId9"/>
-    <hyperlink ref="U4" r:id="rId10"/>
-    <hyperlink ref="F5" r:id="rId11"/>
-    <hyperlink ref="U5" r:id="rId12"/>
-    <hyperlink ref="F9" r:id="rId13"/>
-    <hyperlink ref="F10" r:id="rId14"/>
-    <hyperlink ref="F11" r:id="rId15"/>
-    <hyperlink ref="F12" r:id="rId16"/>
-    <hyperlink ref="F13" r:id="rId17"/>
-    <hyperlink ref="I13" r:id="rId18" location="@lounge.jpg"/>
-    <hyperlink ref="W13" r:id="rId19"/>
-    <hyperlink ref="F14" r:id="rId20"/>
-    <hyperlink ref="X14" r:id="rId21"/>
-    <hyperlink ref="AA14" r:id="rId22"/>
-    <hyperlink ref="AL14" r:id="rId23"/>
-    <hyperlink ref="AN14" r:id="rId24"/>
-    <hyperlink ref="AO14" r:id="rId25"/>
-    <hyperlink ref="AP14" r:id="rId26"/>
-    <hyperlink ref="BA14" r:id="rId27"/>
-    <hyperlink ref="F15" r:id="rId28"/>
-    <hyperlink ref="X15" r:id="rId29"/>
-    <hyperlink ref="Q16" r:id="rId30" location="@lounge.jpg"/>
-    <hyperlink ref="BN16" r:id="rId31" location="@Ebay@#@23.50&amp;euro;@###@https://testing.xataka.com@#@Xataka@#@15,670&amp;euro;"/>
-    <hyperlink ref="BS16" r:id="rId32"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="I2" r:id="rId2" location="@lounge.jpg" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="O2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="Q2" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="X2" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="AB2" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="F3" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="X3" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="F4" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="U4" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="F5" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="U5" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="F9" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="F10" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="F11" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="F12" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="F13" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="I13" r:id="rId18" location="@lounge.jpg" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="W13" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="F14" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="X14" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="AA14" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="AL14" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="AN14" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="AO14" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="AP14" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="BA14" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="F15" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="X15" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="Q16" r:id="rId30" location="@lounge.jpg" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="BN16" r:id="rId31" location="@Ebay@#@23.50&amp;euro;@###@https://testing.xataka.com@#@Xataka@#@15,670&amp;euro;" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="BS16" r:id="rId32" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -9732,7 +9803,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:78" ht="15.75" customHeight="1">
       <c r="A1" s="34" t="s">
@@ -10126,20 +10197,20 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="F2" r:id="rId2"/>
-    <hyperlink ref="H2" r:id="rId3" location="#@http://www.amazon.in/Forzza-Daniel-Large-Finish-Wenge/dp/B01ELJQSS8@##@http://www.amazon.in/Nubia-Z11-Mini-Gold/dp/B01N6MTTV8@##@http://www.amazon.in/Samsung-Z2-SM-Z200F-Gold-8GB/dp/B01LW4PPFV"/>
-    <hyperlink ref="J2" r:id="rId4"/>
-    <hyperlink ref="K2" r:id="rId5"/>
-    <hyperlink ref="H3" r:id="rId6" location="#@http://www.amazon.in/Forzza-Daniel-Large-Finish-Wenge/dp/B01ELJQSS8@##@http://www.amazon.in/Nubia-Z11-Mini-Gold/dp/B01N6MTTV8@##@http://www.amazon.in/Samsung-Z2-SM-Z200F-Gold-8GB/dp/B01LW4PPFV"/>
-    <hyperlink ref="W3" r:id="rId7"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="H2" r:id="rId3" location="#@http://www.amazon.in/Forzza-Daniel-Large-Finish-Wenge/dp/B01ELJQSS8@##@http://www.amazon.in/Nubia-Z11-Mini-Gold/dp/B01N6MTTV8@##@http://www.amazon.in/Samsung-Z2-SM-Z200F-Gold-8GB/dp/B01LW4PPFV" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="J2" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="K2" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="H3" r:id="rId6" location="#@http://www.amazon.in/Forzza-Daniel-Large-Finish-Wenge/dp/B01ELJQSS8@##@http://www.amazon.in/Nubia-Z11-Mini-Gold/dp/B01N6MTTV8@##@http://www.amazon.in/Samsung-Z2-SM-Z200F-Gold-8GB/dp/B01LW4PPFV" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="W3" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -10149,13 +10220,13 @@
       <selection activeCell="CK2" sqref="CK2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="85" max="85" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="86" max="86" width="35.7109375" customWidth="1" collapsed="1"/>
+    <col min="85" max="85" width="27.5" customWidth="1" collapsed="1"/>
+    <col min="86" max="86" width="35.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" ht="63">
+    <row r="1" spans="1:94" ht="64">
       <c r="A1" s="54" t="s">
         <v>16</v>
       </c>
@@ -10414,29 +10485,29 @@
       <c r="CH1" s="58" t="s">
         <v>306</v>
       </c>
-      <c r="CI1" s="119" t="s">
+      <c r="CI1" s="117" t="s">
+        <v>579</v>
+      </c>
+      <c r="CJ1" s="117" t="s">
+        <v>580</v>
+      </c>
+      <c r="CK1" s="55" t="s">
+        <v>581</v>
+      </c>
+      <c r="CL1" s="55" t="s">
+        <v>582</v>
+      </c>
+      <c r="CM1" s="55" t="s">
+        <v>583</v>
+      </c>
+      <c r="CN1" s="55" t="s">
+        <v>584</v>
+      </c>
+      <c r="CO1" s="55" t="s">
         <v>585</v>
       </c>
-      <c r="CJ1" s="119" t="s">
+      <c r="CP1" s="55" t="s">
         <v>586</v>
-      </c>
-      <c r="CK1" s="55" t="s">
-        <v>587</v>
-      </c>
-      <c r="CL1" s="55" t="s">
-        <v>588</v>
-      </c>
-      <c r="CM1" s="55" t="s">
-        <v>589</v>
-      </c>
-      <c r="CN1" s="55" t="s">
-        <v>590</v>
-      </c>
-      <c r="CO1" s="55" t="s">
-        <v>591</v>
-      </c>
-      <c r="CP1" s="55" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="2" spans="1:94" ht="15.75" customHeight="1">
@@ -10698,328 +10769,636 @@
       <c r="CH2" s="71" t="s">
         <v>177</v>
       </c>
-      <c r="CI2" s="120" t="s">
-        <v>177</v>
-      </c>
-      <c r="CJ2" s="120" t="s">
-        <v>198</v>
-      </c>
-      <c r="CK2" s="121" t="s">
-        <v>593</v>
-      </c>
-      <c r="CL2" s="120" t="s">
-        <v>594</v>
-      </c>
-      <c r="CM2" s="122" t="s">
-        <v>595</v>
-      </c>
-      <c r="CN2" s="123" t="s">
-        <v>596</v>
-      </c>
-      <c r="CO2" s="121" t="s">
-        <v>598</v>
-      </c>
-      <c r="CP2" s="121" t="s">
-        <v>597</v>
+      <c r="CI2" s="118" t="s">
+        <v>177</v>
+      </c>
+      <c r="CJ2" s="118" t="s">
+        <v>198</v>
+      </c>
+      <c r="CK2" s="119" t="s">
+        <v>587</v>
+      </c>
+      <c r="CL2" s="118" t="s">
+        <v>588</v>
+      </c>
+      <c r="CM2" s="120" t="s">
+        <v>589</v>
+      </c>
+      <c r="CN2" s="121" t="s">
+        <v>590</v>
+      </c>
+      <c r="CO2" s="119" t="s">
+        <v>592</v>
+      </c>
+      <c r="CP2" s="119" t="s">
+        <v>591</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q2" r:id="rId1" location="@lounge.jpg"/>
-    <hyperlink ref="BS2" r:id="rId2"/>
-    <hyperlink ref="F2" r:id="rId3"/>
-    <hyperlink ref="CM2" r:id="rId4"/>
+    <hyperlink ref="Q2" r:id="rId1" location="@lounge.jpg" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="BS2" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="CM2" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:CL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.83203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="20" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="16" customWidth="1" collapsed="1"/>
     <col min="13" max="14" width="18" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="16.42578125" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="13.85546875" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="16.5" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="21.33203125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.1640625" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.83203125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="17.1640625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="21.33203125" customWidth="1" collapsed="1"/>
     <col min="21" max="21" width="24" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="27.5" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="15.83203125" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="16.6640625" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="15.5" customWidth="1" collapsed="1"/>
     <col min="26" max="26" width="19" customWidth="1" collapsed="1"/>
     <col min="28" max="28" width="14" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.140625" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="14.7109375" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="14.1640625" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="17.1640625" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="14.6640625" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="14.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="106" customFormat="1" ht="45" customHeight="1">
-      <c r="A1" s="54" t="s">
+    <row r="1" spans="1:90" s="105" customFormat="1" ht="45" customHeight="1">
+      <c r="A1" s="134" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="134" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="134" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="54" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="54" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="54" t="s">
+      <c r="D1" s="134" t="s">
+        <v>593</v>
+      </c>
+      <c r="E1" s="134" t="s">
+        <v>594</v>
+      </c>
+      <c r="F1" s="134" t="s">
+        <v>595</v>
+      </c>
+      <c r="G1" s="134" t="s">
+        <v>449</v>
+      </c>
+      <c r="H1" s="134" t="s">
+        <v>596</v>
+      </c>
+      <c r="I1" s="134" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="134" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" s="134" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="134" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="134" t="s">
+        <v>31</v>
+      </c>
+      <c r="N1" s="134" t="s">
+        <v>32</v>
+      </c>
+      <c r="O1" s="134" t="s">
+        <v>33</v>
+      </c>
+      <c r="P1" s="134" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" s="134" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="R1" s="134" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="S1" s="134" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" s="134" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="U1" s="134" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="54" t="s">
+      <c r="V1" s="134" t="s">
         <v>40</v>
       </c>
-      <c r="L1" s="54" t="s">
+      <c r="W1" s="134" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="X1" s="134" t="s">
         <v>42</v>
       </c>
-      <c r="N1" s="54" t="s">
+      <c r="Y1" s="134" t="s">
+        <v>597</v>
+      </c>
+      <c r="Z1" s="134" t="s">
         <v>43</v>
       </c>
-      <c r="O1" s="54" t="s">
+      <c r="AA1" s="134" t="s">
         <v>44</v>
       </c>
-      <c r="P1" s="54" t="s">
+      <c r="AB1" s="134" t="s">
         <v>45</v>
       </c>
-      <c r="Q1" s="56" t="s">
+      <c r="AC1" s="134" t="s">
         <v>115</v>
       </c>
-      <c r="R1" s="56" t="s">
+      <c r="AD1" s="134" t="s">
         <v>116</v>
       </c>
-      <c r="S1" s="105" t="s">
+      <c r="AE1" s="134" t="s">
         <v>126</v>
       </c>
-      <c r="T1" s="56" t="s">
+      <c r="AF1" s="134" t="s">
         <v>127</v>
       </c>
-      <c r="U1" s="56" t="s">
+      <c r="AG1" s="134" t="s">
         <v>128</v>
       </c>
-      <c r="V1" s="56" t="s">
+      <c r="AH1" s="134" t="s">
         <v>129</v>
       </c>
-      <c r="W1" s="56" t="s">
+      <c r="AI1" s="134" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ1" s="134" t="s">
+        <v>131</v>
+      </c>
+      <c r="AK1" s="134" t="s">
+        <v>132</v>
+      </c>
+      <c r="AL1" s="134" t="s">
+        <v>133</v>
+      </c>
+      <c r="AM1" s="134" t="s">
+        <v>134</v>
+      </c>
+      <c r="AN1" s="134" t="s">
+        <v>135</v>
+      </c>
+      <c r="AO1" s="134" t="s">
+        <v>136</v>
+      </c>
+      <c r="AP1" s="134" t="s">
+        <v>137</v>
+      </c>
+      <c r="AQ1" s="134" t="s">
+        <v>138</v>
+      </c>
+      <c r="AR1" s="134" t="s">
+        <v>139</v>
+      </c>
+      <c r="AS1" s="134" t="s">
+        <v>140</v>
+      </c>
+      <c r="AT1" s="134" t="s">
+        <v>141</v>
+      </c>
+      <c r="AU1" s="134" t="s">
+        <v>142</v>
+      </c>
+      <c r="AV1" s="134" t="s">
+        <v>143</v>
+      </c>
+      <c r="AW1" s="134" t="s">
+        <v>144</v>
+      </c>
+      <c r="AX1" s="134" t="s">
+        <v>145</v>
+      </c>
+      <c r="AY1" s="134" t="s">
+        <v>146</v>
+      </c>
+      <c r="AZ1" s="134" t="s">
+        <v>147</v>
+      </c>
+      <c r="BA1" s="134" t="s">
+        <v>148</v>
+      </c>
+      <c r="BB1" s="134" t="s">
+        <v>149</v>
+      </c>
+      <c r="BC1" s="134" t="s">
+        <v>150</v>
+      </c>
+      <c r="BD1" s="134" t="s">
+        <v>151</v>
+      </c>
+      <c r="BE1" s="134" t="s">
+        <v>152</v>
+      </c>
+      <c r="BF1" s="134" t="s">
+        <v>153</v>
+      </c>
+      <c r="BG1" s="134" t="s">
+        <v>154</v>
+      </c>
+      <c r="BH1" s="134" t="s">
+        <v>155</v>
+      </c>
+      <c r="BI1" s="134" t="s">
+        <v>293</v>
+      </c>
+      <c r="BJ1" s="134" t="s">
+        <v>294</v>
+      </c>
+      <c r="BK1" s="134" t="s">
+        <v>295</v>
+      </c>
+      <c r="BL1" s="134" t="s">
+        <v>296</v>
+      </c>
+      <c r="BM1" s="134" t="s">
+        <v>297</v>
+      </c>
+      <c r="BN1" s="134" t="s">
+        <v>298</v>
+      </c>
+      <c r="BO1" s="134" t="s">
+        <v>305</v>
+      </c>
+      <c r="BP1" s="134" t="s">
+        <v>306</v>
+      </c>
+      <c r="BQ1" s="134" t="s">
+        <v>598</v>
+      </c>
+      <c r="BR1" s="134" t="s">
+        <v>599</v>
+      </c>
+      <c r="BS1" s="134" t="s">
+        <v>600</v>
+      </c>
+      <c r="BT1" s="134" t="s">
         <v>156</v>
       </c>
-      <c r="X1" s="56" t="s">
+      <c r="BU1" s="134" t="s">
         <v>157</v>
       </c>
-      <c r="Y1" s="56" t="s">
+      <c r="BV1" s="134" t="s">
+        <v>158</v>
+      </c>
+      <c r="BW1" s="134" t="s">
+        <v>601</v>
+      </c>
+      <c r="BX1" s="134" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="56" t="s">
+      <c r="BY1" s="134" t="s">
         <v>159</v>
       </c>
-      <c r="AA1" s="56" t="s">
+      <c r="BZ1" s="134" t="s">
         <v>47</v>
       </c>
-      <c r="AB1" s="56" t="s">
+      <c r="CA1" s="134" t="s">
         <v>160</v>
       </c>
-      <c r="AC1" s="56" t="s">
+      <c r="CB1" s="134" t="s">
         <v>161</v>
       </c>
-      <c r="AD1" s="56" t="s">
+      <c r="CC1" s="134" t="s">
         <v>162</v>
       </c>
-      <c r="AE1" s="56" t="s">
+      <c r="CD1" s="134" t="s">
         <v>163</v>
       </c>
-      <c r="AF1" s="56" t="s">
+      <c r="CE1" s="134" t="s">
         <v>164</v>
       </c>
-      <c r="AG1" s="56" t="s">
+      <c r="CF1" s="134" t="s">
         <v>165</v>
       </c>
-      <c r="AH1" s="56" t="s">
+      <c r="CG1" s="134" t="s">
         <v>166</v>
       </c>
-      <c r="AI1" s="56" t="s">
+      <c r="CH1" s="134" t="s">
+        <v>602</v>
+      </c>
+      <c r="CI1" s="134" t="s">
         <v>167</v>
       </c>
-      <c r="AJ1" s="56" t="s">
+      <c r="CJ1" s="134" t="s">
         <v>168</v>
       </c>
-      <c r="AK1" s="56" t="s">
+      <c r="CK1" s="134" t="s">
         <v>169</v>
       </c>
-      <c r="AL1" s="56" t="s">
+      <c r="CL1" s="134" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="15.75" customHeight="1">
-      <c r="A2" s="60" t="s">
-        <v>579</v>
-      </c>
-      <c r="B2" s="61" t="s">
-        <v>580</v>
-      </c>
-      <c r="C2" s="63" t="s">
-        <v>582</v>
-      </c>
-      <c r="D2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="E2" s="104" t="s">
-        <v>177</v>
-      </c>
-      <c r="F2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="G2" s="107" t="s">
-        <v>584</v>
-      </c>
-      <c r="H2" s="65" t="s">
-        <v>583</v>
+    <row r="2" spans="1:90" ht="15.75" customHeight="1">
+      <c r="A2" s="135" t="s">
+        <v>603</v>
+      </c>
+      <c r="B2" s="136" t="s">
+        <v>604</v>
+      </c>
+      <c r="C2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" s="136" t="s">
+        <v>449</v>
+      </c>
+      <c r="E2" s="137" t="s">
+        <v>605</v>
+      </c>
+      <c r="F2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" s="137" t="s">
+        <v>606</v>
+      </c>
+      <c r="H2" s="137" t="s">
+        <v>177</v>
       </c>
       <c r="I2" s="136" t="s">
-        <v>581</v>
-      </c>
-      <c r="J2" s="63" t="s">
-        <v>599</v>
-      </c>
-      <c r="K2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="L2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="M2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="N2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="O2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="P2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="R2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="S2" s="63" t="s">
-        <v>179</v>
-      </c>
-      <c r="T2" s="63" t="s">
-        <v>179</v>
-      </c>
-      <c r="U2" s="63" t="s">
-        <v>179</v>
-      </c>
-      <c r="V2" s="63" t="s">
-        <v>179</v>
-      </c>
-      <c r="W2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="X2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="Y2" s="69" t="s">
-        <v>188</v>
-      </c>
-      <c r="Z2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="AA2" s="70" t="s">
-        <v>220</v>
-      </c>
-      <c r="AB2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="AC2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="AD2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="AE2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="AF2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="AG2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="AH2" s="63" t="s">
-        <v>197</v>
-      </c>
-      <c r="AI2" s="63" t="s">
-        <v>177</v>
-      </c>
-      <c r="AJ2" s="63" t="s">
-        <v>198</v>
-      </c>
-      <c r="AK2" s="63" t="s">
-        <v>179</v>
-      </c>
-      <c r="AL2" s="71" t="s">
+        <v>177</v>
+      </c>
+      <c r="J2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="K2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="L2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="M2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="N2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="O2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="P2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q2" s="136" t="s">
+        <v>607</v>
+      </c>
+      <c r="R2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="S2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="T2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="U2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="V2" s="137" t="s">
+        <v>58</v>
+      </c>
+      <c r="W2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="X2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="Y2" s="136" t="s">
+        <v>608</v>
+      </c>
+      <c r="Z2" s="138" t="s">
+        <v>609</v>
+      </c>
+      <c r="AA2" s="136" t="s">
+        <v>610</v>
+      </c>
+      <c r="AB2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AC2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AE2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AG2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AI2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AL2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AM2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AN2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AO2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AP2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AQ2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AR2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AS2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AT2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AU2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AV2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AW2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AX2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AY2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="AZ2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BA2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BB2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BC2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BD2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BE2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BF2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BG2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BH2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BI2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BJ2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BK2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BL2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BM2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BN2" s="136" t="s">
+        <v>611</v>
+      </c>
+      <c r="BO2" s="137" t="s">
+        <v>612</v>
+      </c>
+      <c r="BP2" s="136" t="s">
+        <v>184</v>
+      </c>
+      <c r="BQ2" s="139" t="s">
+        <v>613</v>
+      </c>
+      <c r="BR2" s="136" t="s">
+        <v>614</v>
+      </c>
+      <c r="BS2" s="137" t="s">
+        <v>615</v>
+      </c>
+      <c r="BT2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BU2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BV2" s="140" t="s">
+        <v>616</v>
+      </c>
+      <c r="BW2" s="136" t="s">
+        <v>617</v>
+      </c>
+      <c r="BX2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BY2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="BZ2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="CA2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="CB2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="CC2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="CD2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="CE2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="CF2" s="138" t="s">
+        <v>618</v>
+      </c>
+      <c r="CG2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="CH2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="CI2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="CJ2" s="136" t="s">
+        <v>198</v>
+      </c>
+      <c r="CK2" s="136" t="s">
+        <v>177</v>
+      </c>
+      <c r="CL2" s="136" t="s">
         <v>177</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="Y2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2" display="https://www.youtube.com/embed/Ce7dDso0TfU"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -11027,7 +11406,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="51" t="s">
@@ -11079,17 +11458,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A5" r:id="rId3"/>
-    <hyperlink ref="A6" r:id="rId4"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="A5" r:id="rId3" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="A6" r:id="rId4" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -11097,7 +11476,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1">
       <c r="A1" s="80" t="s">
@@ -11109,13 +11488,13 @@
       <c r="C1" s="81" t="s">
         <v>407</v>
       </c>
-      <c r="D1" s="124" t="s">
+      <c r="D1" s="122" t="s">
         <v>413</v>
       </c>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="126"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="123"/>
+      <c r="H1" s="124"/>
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
       <c r="K1" s="25"/>
@@ -12056,7 +12435,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -12066,7 +12445,7 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" customHeight="1">
       <c r="A1" s="94" t="s">
@@ -12081,42 +12460,42 @@
       <c r="D1" s="95" t="s">
         <v>514</v>
       </c>
-      <c r="E1" s="130" t="s">
+      <c r="E1" s="128" t="s">
         <v>518</v>
       </c>
-      <c r="F1" s="131"/>
-      <c r="G1" s="131"/>
+      <c r="F1" s="129"/>
+      <c r="G1" s="129"/>
       <c r="H1" s="96"/>
-      <c r="I1" s="132" t="s">
+      <c r="I1" s="130" t="s">
         <v>522</v>
       </c>
-      <c r="J1" s="131"/>
-      <c r="K1" s="131"/>
-      <c r="L1" s="133"/>
-      <c r="M1" s="134" t="s">
+      <c r="J1" s="129"/>
+      <c r="K1" s="129"/>
+      <c r="L1" s="131"/>
+      <c r="M1" s="132" t="s">
         <v>526</v>
       </c>
-      <c r="N1" s="128"/>
-      <c r="O1" s="128"/>
-      <c r="P1" s="129"/>
-      <c r="Q1" s="127" t="s">
+      <c r="N1" s="126"/>
+      <c r="O1" s="126"/>
+      <c r="P1" s="127"/>
+      <c r="Q1" s="125" t="s">
         <v>530</v>
       </c>
-      <c r="R1" s="128"/>
-      <c r="S1" s="128"/>
-      <c r="T1" s="129"/>
-      <c r="U1" s="135" t="s">
+      <c r="R1" s="126"/>
+      <c r="S1" s="126"/>
+      <c r="T1" s="127"/>
+      <c r="U1" s="133" t="s">
         <v>533</v>
       </c>
-      <c r="V1" s="128"/>
-      <c r="W1" s="128"/>
-      <c r="X1" s="129"/>
-      <c r="Y1" s="127" t="s">
+      <c r="V1" s="126"/>
+      <c r="W1" s="126"/>
+      <c r="X1" s="127"/>
+      <c r="Y1" s="125" t="s">
         <v>535</v>
       </c>
-      <c r="Z1" s="128"/>
-      <c r="AA1" s="128"/>
-      <c r="AB1" s="129"/>
+      <c r="Z1" s="126"/>
+      <c r="AA1" s="126"/>
+      <c r="AB1" s="127"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="94" t="s">
@@ -12205,1290 +12584,1290 @@
       </c>
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A3" s="108" t="s">
+      <c r="A3" s="106" t="s">
         <v>560</v>
       </c>
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="106" t="s">
         <v>561</v>
       </c>
-      <c r="C3" s="108" t="s">
+      <c r="C3" s="106" t="s">
         <v>562</v>
       </c>
-      <c r="D3" s="109" t="s">
+      <c r="D3" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="E3" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="F3" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="G3" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="H3" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="I3" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="J3" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="K3" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="L3" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="M3" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="N3" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="O3" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="P3" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q3" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="R3" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="S3" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="T3" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="U3" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="V3" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="W3" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="X3" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y3" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z3" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA3" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB3" s="111" t="s">
+      <c r="E3" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="F3" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="G3" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="H3" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="I3" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="J3" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="K3" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="L3" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="M3" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="N3" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="O3" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="P3" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q3" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="R3" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="S3" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="T3" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="U3" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="V3" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="W3" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="X3" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y3" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z3" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA3" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB3" s="109" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A4" s="108" t="s">
+      <c r="A4" s="106" t="s">
         <v>560</v>
       </c>
-      <c r="B4" s="108" t="s">
+      <c r="B4" s="106" t="s">
         <v>561</v>
       </c>
-      <c r="C4" s="108" t="s">
+      <c r="C4" s="106" t="s">
         <v>563</v>
       </c>
-      <c r="D4" s="109" t="s">
+      <c r="D4" s="107" t="s">
         <v>564</v>
       </c>
-      <c r="E4" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="F4" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="G4" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="H4" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="I4" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="J4" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="K4" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="L4" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="M4" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="N4" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="O4" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="P4" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q4" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="R4" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="S4" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="T4" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="U4" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="V4" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="W4" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="X4" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y4" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z4" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA4" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB4" s="111" t="s">
+      <c r="E4" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="F4" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="G4" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="H4" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="I4" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="J4" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="K4" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="L4" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="M4" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="N4" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="O4" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="P4" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q4" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="R4" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="S4" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="T4" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="U4" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="V4" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="W4" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="X4" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y4" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z4" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA4" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB4" s="109" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A5" s="108" t="s">
+      <c r="A5" s="106" t="s">
         <v>560</v>
       </c>
-      <c r="B5" s="108" t="s">
+      <c r="B5" s="106" t="s">
         <v>561</v>
       </c>
-      <c r="C5" s="108" t="s">
+      <c r="C5" s="106" t="s">
         <v>565</v>
       </c>
-      <c r="D5" s="109" t="s">
+      <c r="D5" s="107" t="s">
         <v>566</v>
       </c>
-      <c r="E5" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="F5" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="G5" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="H5" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="I5" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="J5" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="K5" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="L5" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="M5" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="N5" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="O5" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="P5" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q5" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="R5" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="S5" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="T5" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="U5" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="V5" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="W5" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="X5" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y5" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z5" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA5" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="AB5" s="111" t="s">
+      <c r="E5" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="F5" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="G5" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="H5" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="I5" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="J5" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="K5" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="L5" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="M5" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="N5" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="O5" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="P5" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q5" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="R5" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="S5" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="T5" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="U5" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="V5" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="W5" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="X5" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y5" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z5" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA5" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB5" s="109" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A6" s="108" t="s">
+      <c r="A6" s="106" t="s">
         <v>560</v>
       </c>
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="106" t="s">
         <v>561</v>
       </c>
-      <c r="C6" s="108" t="s">
+      <c r="C6" s="106" t="s">
         <v>567</v>
       </c>
-      <c r="D6" s="109" t="s">
+      <c r="D6" s="107" t="s">
         <v>568</v>
       </c>
-      <c r="E6" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="F6" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="G6" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="H6" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="I6" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="J6" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="K6" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="L6" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="M6" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="N6" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="O6" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="P6" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q6" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="R6" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="S6" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="T6" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="U6" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="V6" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="W6" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="X6" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Y6" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z6" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA6" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB6" s="111" t="s">
+      <c r="E6" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="F6" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="G6" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="H6" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="I6" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="J6" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="K6" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="L6" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="M6" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="N6" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="O6" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="P6" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q6" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="R6" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="S6" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="T6" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="U6" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="V6" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="W6" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="X6" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y6" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z6" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA6" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB6" s="109" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A7" s="108" t="s">
+      <c r="A7" s="106" t="s">
         <v>569</v>
       </c>
-      <c r="B7" s="108" t="s">
+      <c r="B7" s="106" t="s">
         <v>561</v>
       </c>
-      <c r="C7" s="108" t="s">
+      <c r="C7" s="106" t="s">
         <v>567</v>
       </c>
-      <c r="D7" s="109" t="s">
+      <c r="D7" s="107" t="s">
         <v>570</v>
       </c>
-      <c r="E7" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="F7" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="G7" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="H7" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="I7" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="J7" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="K7" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="L7" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="M7" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="N7" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="O7" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="P7" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q7" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="R7" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="S7" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="T7" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="U7" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="V7" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="W7" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="X7" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y7" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z7" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA7" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB7" s="111" t="s">
+      <c r="E7" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="F7" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="G7" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="H7" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="I7" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="J7" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="K7" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="L7" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="M7" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="N7" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="O7" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="P7" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q7" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="R7" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="S7" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="T7" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="U7" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="V7" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="W7" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="X7" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y7" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z7" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA7" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB7" s="109" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A8" s="108" t="s">
+      <c r="A8" s="106" t="s">
         <v>571</v>
       </c>
-      <c r="B8" s="108" t="s">
+      <c r="B8" s="106" t="s">
         <v>169</v>
       </c>
-      <c r="C8" s="108" t="s">
+      <c r="C8" s="106" t="s">
         <v>562</v>
       </c>
-      <c r="D8" s="109" t="s">
+      <c r="D8" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="E8" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="F8" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="G8" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="H8" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="I8" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="J8" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="K8" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="L8" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="M8" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="N8" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="O8" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="P8" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q8" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="R8" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="S8" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="T8" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="U8" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="V8" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="W8" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="X8" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y8" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z8" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA8" s="113"/>
-      <c r="AB8" s="111" t="s">
+      <c r="E8" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="F8" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="G8" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="H8" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="I8" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="J8" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="K8" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="L8" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="M8" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="N8" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="O8" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="P8" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q8" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="R8" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="S8" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="T8" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="U8" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="V8" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="W8" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="X8" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y8" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z8" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA8" s="111"/>
+      <c r="AB8" s="109" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A9" s="114" t="s">
+      <c r="A9" s="112" t="s">
         <v>571</v>
       </c>
-      <c r="B9" s="114" t="s">
+      <c r="B9" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="C9" s="114" t="s">
+      <c r="C9" s="112" t="s">
         <v>563</v>
       </c>
-      <c r="D9" s="115" t="s">
+      <c r="D9" s="113" t="s">
         <v>564</v>
       </c>
-      <c r="E9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="F9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="G9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="H9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="I9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="J9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="K9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="L9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="M9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="N9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="O9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="P9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="R9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="S9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="T9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="U9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="V9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="W9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="X9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="Y9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z9" s="116" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA9" s="117" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB9" s="116" t="s">
+      <c r="E9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="F9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="G9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="H9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="I9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="J9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="K9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="L9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="M9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="N9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="O9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="P9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="R9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="S9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="T9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="U9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="V9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="W9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="X9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z9" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA9" s="115" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB9" s="114" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A10" s="108" t="s">
+      <c r="A10" s="106" t="s">
         <v>571</v>
       </c>
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="106" t="s">
         <v>169</v>
       </c>
-      <c r="C10" s="108" t="s">
+      <c r="C10" s="106" t="s">
         <v>567</v>
       </c>
-      <c r="D10" s="109" t="s">
+      <c r="D10" s="107" t="s">
         <v>572</v>
       </c>
-      <c r="E10" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="F10" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="G10" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="H10" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="I10" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="J10" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="K10" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="L10" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="M10" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="N10" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="O10" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="P10" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q10" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="R10" s="118" t="s">
-        <v>179</v>
-      </c>
-      <c r="S10" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="T10" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="U10" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="V10" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="W10" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="X10" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y10" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z10" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA10" s="118" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB10" s="111" t="s">
+      <c r="E10" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="G10" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="H10" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="I10" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="J10" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="K10" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="L10" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="M10" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="N10" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="O10" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="P10" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q10" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="R10" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="S10" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="T10" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="U10" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="V10" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="W10" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="X10" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y10" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z10" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA10" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB10" s="109" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A11" s="108" t="s">
+      <c r="A11" s="106" t="s">
         <v>571</v>
       </c>
-      <c r="B11" s="108" t="s">
+      <c r="B11" s="106" t="s">
         <v>169</v>
       </c>
-      <c r="C11" s="108" t="s">
+      <c r="C11" s="106" t="s">
         <v>565</v>
       </c>
-      <c r="D11" s="109" t="s">
+      <c r="D11" s="107" t="s">
         <v>566</v>
       </c>
-      <c r="E11" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="F11" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="G11" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="H11" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="I11" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="J11" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="K11" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="L11" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="M11" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="N11" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="O11" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="P11" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q11" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="R11" s="118" t="s">
-        <v>179</v>
-      </c>
-      <c r="S11" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="T11" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="U11" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="V11" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="W11" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="X11" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y11" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z11" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA11" s="118" t="s">
-        <v>198</v>
-      </c>
-      <c r="AB11" s="111" t="s">
+      <c r="E11" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="F11" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="G11" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="H11" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="I11" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="J11" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="K11" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="L11" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="M11" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="N11" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="O11" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="P11" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q11" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="R11" s="116" t="s">
+        <v>179</v>
+      </c>
+      <c r="S11" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="T11" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="U11" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="V11" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="W11" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="X11" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y11" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z11" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA11" s="116" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB11" s="109" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A12" s="108" t="s">
+      <c r="A12" s="106" t="s">
         <v>573</v>
       </c>
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="C12" s="108" t="s">
+      <c r="C12" s="106" t="s">
         <v>565</v>
       </c>
-      <c r="D12" s="109" t="s">
+      <c r="D12" s="107" t="s">
         <v>566</v>
       </c>
-      <c r="E12" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="F12" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="G12" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="H12" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="I12" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="J12" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="K12" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="L12" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="M12" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="N12" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="O12" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="P12" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q12" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="R12" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="S12" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="T12" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="U12" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="V12" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="W12" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="X12" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y12" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z12" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA12" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB12" s="111" t="s">
+      <c r="E12" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="F12" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="G12" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="H12" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="I12" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="J12" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="K12" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="L12" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="M12" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="N12" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="O12" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="P12" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q12" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="R12" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="S12" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="T12" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="U12" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="V12" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="W12" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="X12" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y12" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z12" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA12" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB12" s="109" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A13" s="108" t="s">
+      <c r="A13" s="106" t="s">
         <v>573</v>
       </c>
-      <c r="B13" s="108" t="s">
+      <c r="B13" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="C13" s="108" t="s">
+      <c r="C13" s="106" t="s">
         <v>567</v>
       </c>
-      <c r="D13" s="109" t="s">
+      <c r="D13" s="107" t="s">
         <v>570</v>
       </c>
-      <c r="E13" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="F13" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="G13" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="H13" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="I13" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="J13" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="K13" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="L13" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="M13" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="N13" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="O13" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="P13" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q13" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="R13" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="S13" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="T13" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="U13" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="V13" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="W13" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="X13" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y13" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z13" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA13" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB13" s="111" t="s">
+      <c r="E13" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="F13" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="G13" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="H13" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="I13" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="J13" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="K13" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="L13" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="M13" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="N13" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="O13" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="P13" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q13" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="R13" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="S13" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="T13" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="U13" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="V13" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="W13" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="X13" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y13" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z13" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA13" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB13" s="109" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A14" s="108" t="s">
+      <c r="A14" s="106" t="s">
         <v>170</v>
       </c>
-      <c r="B14" s="108" t="s">
+      <c r="B14" s="106" t="s">
         <v>170</v>
       </c>
-      <c r="C14" s="108" t="s">
+      <c r="C14" s="106" t="s">
         <v>562</v>
       </c>
-      <c r="D14" s="109" t="s">
+      <c r="D14" s="107" t="s">
         <v>167</v>
       </c>
-      <c r="E14" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="F14" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="G14" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="H14" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="I14" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="J14" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="K14" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="L14" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="M14" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="N14" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="O14" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="P14" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q14" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="R14" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="S14" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="T14" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="U14" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="V14" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="W14" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="X14" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y14" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z14" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA14" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB14" s="111" t="s">
+      <c r="E14" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="F14" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="G14" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="H14" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="I14" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="J14" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="K14" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="L14" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="M14" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="N14" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="O14" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="P14" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q14" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="R14" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="S14" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="T14" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="U14" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="V14" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="W14" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="X14" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y14" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z14" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA14" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB14" s="109" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A15" s="108" t="s">
+      <c r="A15" s="106" t="s">
         <v>170</v>
       </c>
-      <c r="B15" s="108" t="s">
+      <c r="B15" s="106" t="s">
         <v>170</v>
       </c>
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="106" t="s">
         <v>563</v>
       </c>
-      <c r="D15" s="109" t="s">
+      <c r="D15" s="107" t="s">
         <v>574</v>
       </c>
-      <c r="E15" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="F15" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="G15" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="H15" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="I15" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="J15" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="K15" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="L15" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="M15" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="N15" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="O15" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="P15" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q15" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="R15" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="S15" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="T15" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="U15" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="V15" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="W15" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="X15" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y15" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z15" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA15" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB15" s="111" t="s">
+      <c r="E15" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="F15" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="G15" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="H15" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="I15" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="J15" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="K15" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="L15" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="M15" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="N15" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="O15" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="P15" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q15" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="R15" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="S15" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="T15" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="U15" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="V15" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="W15" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="X15" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y15" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z15" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA15" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB15" s="109" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A16" s="108" t="s">
+      <c r="A16" s="106" t="s">
         <v>170</v>
       </c>
-      <c r="B16" s="108" t="s">
+      <c r="B16" s="106" t="s">
         <v>170</v>
       </c>
-      <c r="C16" s="108" t="s">
+      <c r="C16" s="106" t="s">
         <v>565</v>
       </c>
-      <c r="D16" s="109" t="s">
+      <c r="D16" s="107" t="s">
         <v>566</v>
       </c>
-      <c r="E16" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="F16" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="G16" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="H16" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="I16" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="J16" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="K16" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="L16" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="M16" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="N16" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="O16" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="P16" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q16" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="R16" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="S16" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="T16" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="U16" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="V16" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="W16" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="X16" s="112" t="s">
-        <v>198</v>
-      </c>
-      <c r="Y16" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z16" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA16" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="AB16" s="111" t="s">
+      <c r="E16" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="F16" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="G16" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="H16" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="I16" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="J16" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="K16" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="L16" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="M16" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="N16" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="O16" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="P16" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q16" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="R16" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="S16" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="T16" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="U16" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="V16" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="W16" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="X16" s="110" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y16" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z16" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA16" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB16" s="109" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:28" ht="15.75" customHeight="1">
-      <c r="A17" s="108" t="s">
+      <c r="A17" s="106" t="s">
         <v>170</v>
       </c>
-      <c r="B17" s="108" t="s">
+      <c r="B17" s="106" t="s">
         <v>170</v>
       </c>
-      <c r="C17" s="108" t="s">
+      <c r="C17" s="106" t="s">
         <v>575</v>
       </c>
-      <c r="D17" s="109" t="s">
+      <c r="D17" s="107" t="s">
         <v>568</v>
       </c>
-      <c r="E17" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="F17" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="G17" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="H17" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="I17" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="J17" s="111" t="s">
-        <v>198</v>
-      </c>
-      <c r="K17" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="L17" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="M17" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="N17" s="110" t="s">
-        <v>198</v>
-      </c>
-      <c r="O17" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="P17" s="110" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q17" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="R17" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="S17" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="T17" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="U17" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="V17" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="W17" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="X17" s="112" t="s">
-        <v>179</v>
-      </c>
-      <c r="Y17" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z17" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AA17" s="111" t="s">
-        <v>179</v>
-      </c>
-      <c r="AB17" s="111" t="s">
+      <c r="E17" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="F17" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="G17" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="H17" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="I17" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="J17" s="109" t="s">
+        <v>198</v>
+      </c>
+      <c r="K17" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="L17" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="M17" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="N17" s="108" t="s">
+        <v>198</v>
+      </c>
+      <c r="O17" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="P17" s="108" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q17" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="R17" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="S17" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="T17" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="U17" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="V17" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="W17" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="X17" s="110" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y17" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z17" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AA17" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB17" s="109" t="s">
         <v>179</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1. Updated createMVPPostExcel file 2. updated common MVP methods. 3. New common MVP methods.
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/excel.xlsx
+++ b/Aml_automation/src/Common/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isha/git/Automation/Aml_automation/src/Common/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8F02FBD5-B531-974D-AC37-801D930BCBF4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{64E4DC90-1A6A-5E49-942E-DBFEC2D3EEC6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="12440" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1843,9 +1843,6 @@
     <t>brand alfa</t>
   </si>
   <si>
-    <t>Isha alfa</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=p6LcnmsVhc0</t>
   </si>
   <si>
@@ -1886,6 +1883,9 @@
   </si>
   <si>
     <t>https://twitter.com/marcvidal/status/963332880972775424</t>
+  </si>
+  <si>
+    <t>Isha alfa testing</t>
   </si>
 </sst>
 </file>
@@ -3000,6 +3000,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="33" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3024,13 +3031,6 @@
     <xf numFmtId="0" fontId="14" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5387,42 +5387,42 @@
       <c r="C1" s="95" t="s">
         <v>514</v>
       </c>
-      <c r="D1" s="128" t="s">
+      <c r="D1" s="135" t="s">
         <v>518</v>
       </c>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
       <c r="G1" s="96"/>
-      <c r="H1" s="130" t="s">
+      <c r="H1" s="137" t="s">
         <v>522</v>
       </c>
-      <c r="I1" s="129"/>
-      <c r="J1" s="129"/>
-      <c r="K1" s="131"/>
-      <c r="L1" s="132" t="s">
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="138"/>
+      <c r="L1" s="139" t="s">
         <v>526</v>
       </c>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
-      <c r="O1" s="127"/>
-      <c r="P1" s="125" t="s">
+      <c r="M1" s="133"/>
+      <c r="N1" s="133"/>
+      <c r="O1" s="134"/>
+      <c r="P1" s="132" t="s">
         <v>530</v>
       </c>
-      <c r="Q1" s="126"/>
-      <c r="R1" s="126"/>
-      <c r="S1" s="127"/>
-      <c r="T1" s="133" t="s">
+      <c r="Q1" s="133"/>
+      <c r="R1" s="133"/>
+      <c r="S1" s="134"/>
+      <c r="T1" s="140" t="s">
         <v>533</v>
       </c>
-      <c r="U1" s="126"/>
-      <c r="V1" s="126"/>
-      <c r="W1" s="127"/>
-      <c r="X1" s="125" t="s">
+      <c r="U1" s="133"/>
+      <c r="V1" s="133"/>
+      <c r="W1" s="134"/>
+      <c r="X1" s="132" t="s">
         <v>535</v>
       </c>
-      <c r="Y1" s="126"/>
-      <c r="Z1" s="126"/>
-      <c r="AA1" s="127"/>
+      <c r="Y1" s="133"/>
+      <c r="Z1" s="133"/>
+      <c r="AA1" s="134"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1">
       <c r="A2" s="94" t="s">
@@ -10809,8 +10809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:CL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -10848,546 +10848,546 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:90" s="105" customFormat="1" ht="45" customHeight="1">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="134" t="s">
+      <c r="B1" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="134" t="s">
+      <c r="C1" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="134" t="s">
+      <c r="D1" s="122" t="s">
         <v>593</v>
       </c>
-      <c r="E1" s="134" t="s">
+      <c r="E1" s="122" t="s">
         <v>594</v>
       </c>
-      <c r="F1" s="134" t="s">
+      <c r="F1" s="122" t="s">
         <v>595</v>
       </c>
-      <c r="G1" s="134" t="s">
+      <c r="G1" s="122" t="s">
         <v>449</v>
       </c>
-      <c r="H1" s="134" t="s">
+      <c r="H1" s="122" t="s">
         <v>596</v>
       </c>
-      <c r="I1" s="134" t="s">
+      <c r="I1" s="122" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="134" t="s">
+      <c r="J1" s="122" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="134" t="s">
+      <c r="K1" s="122" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="134" t="s">
+      <c r="L1" s="122" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="134" t="s">
+      <c r="M1" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="134" t="s">
+      <c r="N1" s="122" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="134" t="s">
+      <c r="O1" s="122" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="134" t="s">
+      <c r="P1" s="122" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="134" t="s">
+      <c r="Q1" s="122" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="134" t="s">
+      <c r="R1" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="134" t="s">
+      <c r="S1" s="122" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="134" t="s">
+      <c r="T1" s="122" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="134" t="s">
+      <c r="U1" s="122" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="134" t="s">
+      <c r="V1" s="122" t="s">
         <v>40</v>
       </c>
-      <c r="W1" s="134" t="s">
+      <c r="W1" s="122" t="s">
         <v>41</v>
       </c>
-      <c r="X1" s="134" t="s">
+      <c r="X1" s="122" t="s">
         <v>42</v>
       </c>
-      <c r="Y1" s="134" t="s">
+      <c r="Y1" s="122" t="s">
         <v>597</v>
       </c>
-      <c r="Z1" s="134" t="s">
+      <c r="Z1" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" s="134" t="s">
+      <c r="AA1" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="AB1" s="134" t="s">
+      <c r="AB1" s="122" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" s="134" t="s">
+      <c r="AC1" s="122" t="s">
         <v>115</v>
       </c>
-      <c r="AD1" s="134" t="s">
+      <c r="AD1" s="122" t="s">
         <v>116</v>
       </c>
-      <c r="AE1" s="134" t="s">
+      <c r="AE1" s="122" t="s">
         <v>126</v>
       </c>
-      <c r="AF1" s="134" t="s">
+      <c r="AF1" s="122" t="s">
         <v>127</v>
       </c>
-      <c r="AG1" s="134" t="s">
+      <c r="AG1" s="122" t="s">
         <v>128</v>
       </c>
-      <c r="AH1" s="134" t="s">
+      <c r="AH1" s="122" t="s">
         <v>129</v>
       </c>
-      <c r="AI1" s="134" t="s">
+      <c r="AI1" s="122" t="s">
         <v>130</v>
       </c>
-      <c r="AJ1" s="134" t="s">
+      <c r="AJ1" s="122" t="s">
         <v>131</v>
       </c>
-      <c r="AK1" s="134" t="s">
+      <c r="AK1" s="122" t="s">
         <v>132</v>
       </c>
-      <c r="AL1" s="134" t="s">
+      <c r="AL1" s="122" t="s">
         <v>133</v>
       </c>
-      <c r="AM1" s="134" t="s">
+      <c r="AM1" s="122" t="s">
         <v>134</v>
       </c>
-      <c r="AN1" s="134" t="s">
+      <c r="AN1" s="122" t="s">
         <v>135</v>
       </c>
-      <c r="AO1" s="134" t="s">
+      <c r="AO1" s="122" t="s">
         <v>136</v>
       </c>
-      <c r="AP1" s="134" t="s">
+      <c r="AP1" s="122" t="s">
         <v>137</v>
       </c>
-      <c r="AQ1" s="134" t="s">
+      <c r="AQ1" s="122" t="s">
         <v>138</v>
       </c>
-      <c r="AR1" s="134" t="s">
+      <c r="AR1" s="122" t="s">
         <v>139</v>
       </c>
-      <c r="AS1" s="134" t="s">
+      <c r="AS1" s="122" t="s">
         <v>140</v>
       </c>
-      <c r="AT1" s="134" t="s">
+      <c r="AT1" s="122" t="s">
         <v>141</v>
       </c>
-      <c r="AU1" s="134" t="s">
+      <c r="AU1" s="122" t="s">
         <v>142</v>
       </c>
-      <c r="AV1" s="134" t="s">
+      <c r="AV1" s="122" t="s">
         <v>143</v>
       </c>
-      <c r="AW1" s="134" t="s">
+      <c r="AW1" s="122" t="s">
         <v>144</v>
       </c>
-      <c r="AX1" s="134" t="s">
+      <c r="AX1" s="122" t="s">
         <v>145</v>
       </c>
-      <c r="AY1" s="134" t="s">
+      <c r="AY1" s="122" t="s">
         <v>146</v>
       </c>
-      <c r="AZ1" s="134" t="s">
+      <c r="AZ1" s="122" t="s">
         <v>147</v>
       </c>
-      <c r="BA1" s="134" t="s">
+      <c r="BA1" s="122" t="s">
         <v>148</v>
       </c>
-      <c r="BB1" s="134" t="s">
+      <c r="BB1" s="122" t="s">
         <v>149</v>
       </c>
-      <c r="BC1" s="134" t="s">
+      <c r="BC1" s="122" t="s">
         <v>150</v>
       </c>
-      <c r="BD1" s="134" t="s">
+      <c r="BD1" s="122" t="s">
         <v>151</v>
       </c>
-      <c r="BE1" s="134" t="s">
+      <c r="BE1" s="122" t="s">
         <v>152</v>
       </c>
-      <c r="BF1" s="134" t="s">
+      <c r="BF1" s="122" t="s">
         <v>153</v>
       </c>
-      <c r="BG1" s="134" t="s">
+      <c r="BG1" s="122" t="s">
         <v>154</v>
       </c>
-      <c r="BH1" s="134" t="s">
+      <c r="BH1" s="122" t="s">
         <v>155</v>
       </c>
-      <c r="BI1" s="134" t="s">
+      <c r="BI1" s="122" t="s">
         <v>293</v>
       </c>
-      <c r="BJ1" s="134" t="s">
+      <c r="BJ1" s="122" t="s">
         <v>294</v>
       </c>
-      <c r="BK1" s="134" t="s">
+      <c r="BK1" s="122" t="s">
         <v>295</v>
       </c>
-      <c r="BL1" s="134" t="s">
+      <c r="BL1" s="122" t="s">
         <v>296</v>
       </c>
-      <c r="BM1" s="134" t="s">
+      <c r="BM1" s="122" t="s">
         <v>297</v>
       </c>
-      <c r="BN1" s="134" t="s">
+      <c r="BN1" s="122" t="s">
         <v>298</v>
       </c>
-      <c r="BO1" s="134" t="s">
+      <c r="BO1" s="122" t="s">
         <v>305</v>
       </c>
-      <c r="BP1" s="134" t="s">
+      <c r="BP1" s="122" t="s">
         <v>306</v>
       </c>
-      <c r="BQ1" s="134" t="s">
+      <c r="BQ1" s="122" t="s">
         <v>598</v>
       </c>
-      <c r="BR1" s="134" t="s">
+      <c r="BR1" s="122" t="s">
         <v>599</v>
       </c>
-      <c r="BS1" s="134" t="s">
+      <c r="BS1" s="122" t="s">
         <v>600</v>
       </c>
-      <c r="BT1" s="134" t="s">
+      <c r="BT1" s="122" t="s">
         <v>156</v>
       </c>
-      <c r="BU1" s="134" t="s">
+      <c r="BU1" s="122" t="s">
         <v>157</v>
       </c>
-      <c r="BV1" s="134" t="s">
+      <c r="BV1" s="122" t="s">
         <v>158</v>
       </c>
-      <c r="BW1" s="134" t="s">
+      <c r="BW1" s="122" t="s">
         <v>601</v>
       </c>
-      <c r="BX1" s="134" t="s">
+      <c r="BX1" s="122" t="s">
         <v>17</v>
       </c>
-      <c r="BY1" s="134" t="s">
+      <c r="BY1" s="122" t="s">
         <v>159</v>
       </c>
-      <c r="BZ1" s="134" t="s">
+      <c r="BZ1" s="122" t="s">
         <v>47</v>
       </c>
-      <c r="CA1" s="134" t="s">
+      <c r="CA1" s="122" t="s">
         <v>160</v>
       </c>
-      <c r="CB1" s="134" t="s">
+      <c r="CB1" s="122" t="s">
         <v>161</v>
       </c>
-      <c r="CC1" s="134" t="s">
+      <c r="CC1" s="122" t="s">
         <v>162</v>
       </c>
-      <c r="CD1" s="134" t="s">
+      <c r="CD1" s="122" t="s">
         <v>163</v>
       </c>
-      <c r="CE1" s="134" t="s">
+      <c r="CE1" s="122" t="s">
         <v>164</v>
       </c>
-      <c r="CF1" s="134" t="s">
+      <c r="CF1" s="122" t="s">
         <v>165</v>
       </c>
-      <c r="CG1" s="134" t="s">
+      <c r="CG1" s="122" t="s">
         <v>166</v>
       </c>
-      <c r="CH1" s="134" t="s">
+      <c r="CH1" s="122" t="s">
         <v>602</v>
       </c>
-      <c r="CI1" s="134" t="s">
+      <c r="CI1" s="122" t="s">
         <v>167</v>
       </c>
-      <c r="CJ1" s="134" t="s">
+      <c r="CJ1" s="122" t="s">
         <v>168</v>
       </c>
-      <c r="CK1" s="134" t="s">
+      <c r="CK1" s="122" t="s">
         <v>169</v>
       </c>
-      <c r="CL1" s="134" t="s">
+      <c r="CL1" s="122" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="2" spans="1:90" ht="15.75" customHeight="1">
-      <c r="A2" s="135" t="s">
+      <c r="A2" s="123" t="s">
         <v>603</v>
       </c>
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="124" t="s">
+        <v>618</v>
+      </c>
+      <c r="C2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" s="124" t="s">
+        <v>449</v>
+      </c>
+      <c r="E2" s="125" t="s">
         <v>604</v>
       </c>
-      <c r="C2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="D2" s="136" t="s">
-        <v>449</v>
-      </c>
-      <c r="E2" s="137" t="s">
+      <c r="F2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="G2" s="125" t="s">
         <v>605</v>
       </c>
-      <c r="F2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="G2" s="137" t="s">
+      <c r="H2" s="125" t="s">
+        <v>177</v>
+      </c>
+      <c r="I2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="J2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="K2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="L2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="M2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="N2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="O2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="P2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q2" s="124" t="s">
         <v>606</v>
       </c>
-      <c r="H2" s="137" t="s">
-        <v>177</v>
-      </c>
-      <c r="I2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="J2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="K2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="L2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="M2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="N2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="O2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="P2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q2" s="136" t="s">
+      <c r="R2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="S2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="T2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="U2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="V2" s="125" t="s">
+        <v>58</v>
+      </c>
+      <c r="W2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="X2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="Y2" s="124" t="s">
         <v>607</v>
       </c>
-      <c r="R2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="S2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="T2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="U2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="V2" s="137" t="s">
-        <v>58</v>
-      </c>
-      <c r="W2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="X2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="Y2" s="136" t="s">
+      <c r="Z2" s="126" t="s">
         <v>608</v>
       </c>
-      <c r="Z2" s="138" t="s">
+      <c r="AA2" s="124" t="s">
         <v>609</v>
       </c>
-      <c r="AA2" s="136" t="s">
+      <c r="AB2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AC2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AE2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AG2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AI2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AL2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AM2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AN2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AO2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AP2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AQ2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AR2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AS2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AT2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AU2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AV2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AW2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AX2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AY2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="AZ2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BA2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BB2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BC2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BD2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BE2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BF2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BG2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BH2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BI2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BJ2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BK2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BL2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BM2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BN2" s="124" t="s">
         <v>610</v>
       </c>
-      <c r="AB2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AC2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AD2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AE2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AF2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AG2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AH2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AI2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AJ2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AK2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AL2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AM2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AN2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AO2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AP2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AQ2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AR2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AS2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AT2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AU2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AV2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AW2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AX2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AY2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="AZ2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BA2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BB2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BC2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BD2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BE2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BF2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BG2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BH2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BI2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BJ2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BK2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BL2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BM2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BN2" s="136" t="s">
+      <c r="BO2" s="125" t="s">
         <v>611</v>
       </c>
-      <c r="BO2" s="137" t="s">
+      <c r="BP2" s="124" t="s">
+        <v>184</v>
+      </c>
+      <c r="BQ2" s="127" t="s">
         <v>612</v>
       </c>
-      <c r="BP2" s="136" t="s">
-        <v>184</v>
-      </c>
-      <c r="BQ2" s="139" t="s">
+      <c r="BR2" s="124" t="s">
         <v>613</v>
       </c>
-      <c r="BR2" s="136" t="s">
+      <c r="BS2" s="125" t="s">
         <v>614</v>
       </c>
-      <c r="BS2" s="137" t="s">
+      <c r="BT2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BU2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BV2" s="128" t="s">
         <v>615</v>
       </c>
-      <c r="BT2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BU2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BV2" s="140" t="s">
+      <c r="BW2" s="124" t="s">
         <v>616</v>
       </c>
-      <c r="BW2" s="136" t="s">
+      <c r="BX2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BY2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="BZ2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="CA2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="CB2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="CC2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="CD2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="CE2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="CF2" s="126" t="s">
         <v>617</v>
       </c>
-      <c r="BX2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BY2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="BZ2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="CA2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="CB2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="CC2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="CD2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="CE2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="CF2" s="138" t="s">
-        <v>618</v>
-      </c>
-      <c r="CG2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="CH2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="CI2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="CJ2" s="136" t="s">
-        <v>198</v>
-      </c>
-      <c r="CK2" s="136" t="s">
-        <v>177</v>
-      </c>
-      <c r="CL2" s="136" t="s">
+      <c r="CG2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="CH2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="CI2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="CJ2" s="124" t="s">
+        <v>198</v>
+      </c>
+      <c r="CK2" s="124" t="s">
+        <v>177</v>
+      </c>
+      <c r="CL2" s="124" t="s">
         <v>177</v>
       </c>
     </row>
@@ -11488,13 +11488,13 @@
       <c r="C1" s="81" t="s">
         <v>407</v>
       </c>
-      <c r="D1" s="122" t="s">
+      <c r="D1" s="129" t="s">
         <v>413</v>
       </c>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="123"/>
-      <c r="H1" s="124"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="131"/>
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
       <c r="K1" s="25"/>
@@ -12460,42 +12460,42 @@
       <c r="D1" s="95" t="s">
         <v>514</v>
       </c>
-      <c r="E1" s="128" t="s">
+      <c r="E1" s="135" t="s">
         <v>518</v>
       </c>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
       <c r="H1" s="96"/>
-      <c r="I1" s="130" t="s">
+      <c r="I1" s="137" t="s">
         <v>522</v>
       </c>
-      <c r="J1" s="129"/>
-      <c r="K1" s="129"/>
-      <c r="L1" s="131"/>
-      <c r="M1" s="132" t="s">
+      <c r="J1" s="136"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="138"/>
+      <c r="M1" s="139" t="s">
         <v>526</v>
       </c>
-      <c r="N1" s="126"/>
-      <c r="O1" s="126"/>
-      <c r="P1" s="127"/>
-      <c r="Q1" s="125" t="s">
+      <c r="N1" s="133"/>
+      <c r="O1" s="133"/>
+      <c r="P1" s="134"/>
+      <c r="Q1" s="132" t="s">
         <v>530</v>
       </c>
-      <c r="R1" s="126"/>
-      <c r="S1" s="126"/>
-      <c r="T1" s="127"/>
-      <c r="U1" s="133" t="s">
+      <c r="R1" s="133"/>
+      <c r="S1" s="133"/>
+      <c r="T1" s="134"/>
+      <c r="U1" s="140" t="s">
         <v>533</v>
       </c>
-      <c r="V1" s="126"/>
-      <c r="W1" s="126"/>
-      <c r="X1" s="127"/>
-      <c r="Y1" s="125" t="s">
+      <c r="V1" s="133"/>
+      <c r="W1" s="133"/>
+      <c r="X1" s="134"/>
+      <c r="Y1" s="132" t="s">
         <v>535</v>
       </c>
-      <c r="Z1" s="126"/>
-      <c r="AA1" s="126"/>
-      <c r="AB1" s="127"/>
+      <c r="Z1" s="133"/>
+      <c r="AA1" s="133"/>
+      <c r="AB1" s="134"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1">
       <c r="A2" s="94" t="s">

</xml_diff>

<commit_message>
Refined createMVPPostExcel and common MVP methods
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/excel.xlsx
+++ b/Aml_automation/src/Common/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isha/git/Automation/Aml_automation/src/Common/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{64E4DC90-1A6A-5E49-942E-DBFEC2D3EEC6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{27FFF52D-EED7-2F49-AB1B-7BC92D646F08}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="12440" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1885,7 +1885,7 @@
     <t>https://twitter.com/marcvidal/status/963332880972775424</t>
   </si>
   <si>
-    <t>Isha alfa testing</t>
+    <t>Isha alfa test</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
1. New common method MVP_add_fichareview
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/excel.xlsx
+++ b/Aml_automation/src/Common/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isha/git/Automation/Aml_automation/src/Common/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C7BE4D2C-D03B-DB4F-AC6C-16FA31AE9A8E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{695A6EC4-7AE0-E345-AD40-2F3157D82E11}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="12700" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9303,7 +9303,7 @@
   <dimension ref="A1:DE2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="CX1" workbookViewId="0">
-      <selection activeCell="CZ14" sqref="CZ14"/>
+      <selection activeCell="CZ2" sqref="CZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13"/>

</xml_diff>

<commit_message>
updated mvppost excel file
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/excel.xlsx
+++ b/Aml_automation/src/Common/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isha/git/Automation/Aml_automation/src/Common/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2BC02179-8679-EF48-8865-CC028762CF96}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1EACA2D5-D583-9747-8420-123117CD652A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9200" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1986,7 +1986,7 @@
     <t>Destacado</t>
   </si>
   <si>
-    <t>Llevamos años hablando sobre la revolución de la carne de mentira.</t>
+    <t>Llevamos años hablando sobre la revolución de la carne de mentira…</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Refactor Pivot External Alfa and Pivot Insta
</commit_message>
<xml_diff>
--- a/Aml_automation/src/Common/excel.xlsx
+++ b/Aml_automation/src/Common/excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13035" tabRatio="500" activeTab="4"/>
+    <workbookView windowWidth="23985" windowHeight="5445" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TagCatagory" sheetId="1" r:id="rId1"/>
@@ -19,11 +19,12 @@
     <sheet name="Dashboard Programmed Editorial" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <oleSize ref="A1:DB2"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2645" uniqueCount="636">
   <si>
     <t>Blog Name</t>
   </si>
@@ -1520,6 +1521,9 @@
   </si>
   <si>
     <t>flipboard</t>
+  </si>
+  <si>
+    <t>Pivot_Insta</t>
   </si>
   <si>
     <t>alfa</t>
@@ -1983,8 +1987,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="63">
@@ -2266,14 +2270,44 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2288,7 +2322,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2311,15 +2345,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2333,54 +2367,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2394,15 +2381,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2513,19 +2517,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2543,13 +2649,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2567,127 +2685,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3061,23 +3065,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3085,8 +3074,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3121,26 +3121,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -3155,149 +3135,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="52" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="49" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="49" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="49" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="49" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="49" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="20" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="52" fillId="37" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="21" borderId="34" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="46" fillId="38" borderId="34" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="53" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="59" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="60" fillId="47" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="47" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="61" fillId="46" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="57" fillId="46" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="47" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="60" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="53" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="19" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="56" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="59" fillId="19" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="43" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="53" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="45" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="53" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="43" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -5083,46 +5087,46 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:27">
       <c r="A1" s="1" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="4"/>
       <c r="H1" s="5" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="8" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
       <c r="P1" s="9" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="Q1" s="9"/>
       <c r="R1" s="9"/>
       <c r="S1" s="9"/>
       <c r="T1" s="10" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="U1" s="10"/>
       <c r="V1" s="10"/>
       <c r="W1" s="10"/>
       <c r="X1" s="9" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="Y1" s="9"/>
       <c r="Z1" s="9"/>
@@ -5130,85 +5134,85 @@
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:27">
       <c r="A2" s="1" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="U2" s="11" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="V2" s="11" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="W2" s="11" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="X2" s="7" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="Z2" s="7" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="AA2" s="7" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="3" ht="13.5"/>
@@ -9934,10 +9938,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:DB2"/>
+  <dimension ref="A1:DC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CN1" workbookViewId="0">
-      <selection activeCell="DA5" sqref="DA5"/>
+    <sheetView tabSelected="1" topLeftCell="CR1" workbookViewId="0">
+      <selection activeCell="DB9" sqref="DB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="1"/>
@@ -9954,7 +9958,7 @@
     <col min="1024" max="16384" width="9" style="53"/>
   </cols>
   <sheetData>
-    <row r="1" s="51" customFormat="1" ht="63" spans="1:106">
+    <row r="1" s="51" customFormat="1" ht="63" spans="1:107">
       <c r="A1" s="54" t="s">
         <v>260</v>
       </c>
@@ -10273,16 +10277,19 @@
       <c r="DB1" s="71" t="s">
         <v>498</v>
       </c>
+      <c r="DC1" s="71" t="s">
+        <v>499</v>
+      </c>
     </row>
-    <row r="2" s="51" customFormat="1" ht="15.75" customHeight="1" spans="1:106">
+    <row r="2" s="51" customFormat="1" ht="15.75" customHeight="1" spans="1:107">
       <c r="A2" s="56" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C2" s="57" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D2" s="58" t="s">
         <v>341</v>
@@ -10333,10 +10340,10 @@
         <v>341</v>
       </c>
       <c r="T2" s="57" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="U2" s="61" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="V2" s="51" t="s">
         <v>341</v>
@@ -10357,13 +10364,13 @@
         <v>341</v>
       </c>
       <c r="AB2" s="51" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="AC2" s="63" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="AD2" s="51" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="AE2" s="51" t="s">
         <v>341</v>
@@ -10480,7 +10487,7 @@
         <v>341</v>
       </c>
       <c r="BQ2" s="51" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="BR2" s="51" t="s">
         <v>341</v>
@@ -10489,10 +10496,10 @@
         <v>341</v>
       </c>
       <c r="BT2" s="64" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="BU2" s="51" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="BV2" s="51" t="s">
         <v>341</v>
@@ -10519,7 +10526,7 @@
         <v>341</v>
       </c>
       <c r="CD2" s="63" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="CE2" s="51" t="s">
         <v>341</v>
@@ -10549,48 +10556,51 @@
         <v>341</v>
       </c>
       <c r="CN2" s="51" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="CO2" s="51" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="CP2" s="62" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="CQ2" s="51" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="CR2" s="51" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="CS2" s="51" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="CT2" s="66" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="CU2" s="58" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="CV2" s="62" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="CW2" s="67" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="CX2" s="68" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="CY2" s="69" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="CZ2" s="70" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="DA2" s="70" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="DB2" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="DC2" s="51" t="s">
         <v>22</v>
       </c>
     </row>
@@ -10767,21 +10777,21 @@
         <v>480</v>
       </c>
       <c r="AM1" s="50" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="AN1" s="50" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:40">
       <c r="A2" s="39" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="D2" s="41" t="s">
         <v>341</v>
@@ -10793,16 +10803,16 @@
         <v>341</v>
       </c>
       <c r="G2" s="43" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="H2" s="44" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="I2" s="45" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="J2" s="41" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="K2" s="41" t="s">
         <v>341</v>
@@ -10889,10 +10899,10 @@
         <v>341</v>
       </c>
       <c r="AM2" s="51" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="AN2" s="52" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -10923,31 +10933,31 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:2">
       <c r="A1" s="35" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:2">
       <c r="A2" s="36" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:2">
       <c r="A3" s="36" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:2">
       <c r="A4" s="36" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B4" s="35">
         <v>123456</v>
@@ -10955,18 +10965,18 @@
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:2">
       <c r="A5" s="36" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:2">
       <c r="A6" s="36" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
   </sheetData>
@@ -10998,16 +11008,16 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:14">
       <c r="A1" s="23" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>260</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
@@ -11022,28 +11032,28 @@
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:14">
       <c r="A2" s="23" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="B2" s="23" t="s">
         <v>260</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="H2" s="23" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="I2" s="34"/>
       <c r="J2" s="34"/>
@@ -11090,10 +11100,10 @@
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:14">
       <c r="A4" s="25" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C4" s="26">
         <v>0</v>
@@ -11124,10 +11134,10 @@
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:14">
       <c r="A5" s="25" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C5" s="28">
         <v>3</v>
@@ -11158,10 +11168,10 @@
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:14">
       <c r="A6" s="25" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C6" s="26">
         <v>15</v>
@@ -11192,7 +11202,7 @@
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="1:14">
       <c r="A7" s="25" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>15</v>
@@ -11226,10 +11236,10 @@
     </row>
     <row r="8" ht="15.75" customHeight="1" spans="1:14">
       <c r="A8" s="25" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="27" t="s">
@@ -11258,7 +11268,7 @@
     </row>
     <row r="9" ht="15.75" customHeight="1" spans="1:14">
       <c r="A9" s="25" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>15</v>
@@ -11282,10 +11292,10 @@
     </row>
     <row r="10" ht="15.75" customHeight="1" spans="1:14">
       <c r="A10" s="25" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C10" s="29"/>
       <c r="D10" s="30"/>
@@ -11304,7 +11314,7 @@
     </row>
     <row r="11" ht="15.75" customHeight="1" spans="1:14">
       <c r="A11" s="25" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>15</v>
@@ -11338,10 +11348,10 @@
     </row>
     <row r="12" ht="15.75" customHeight="1" spans="1:14">
       <c r="A12" s="25" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C12" s="26">
         <v>18</v>
@@ -11372,7 +11382,7 @@
     </row>
     <row r="13" ht="15.75" customHeight="1" spans="1:14">
       <c r="A13" s="25" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>15</v>
@@ -11404,10 +11414,10 @@
     </row>
     <row r="14" ht="15.75" customHeight="1" spans="1:14">
       <c r="A14" s="25" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C14" s="29"/>
       <c r="D14" s="27" t="s">
@@ -11470,7 +11480,7 @@
     </row>
     <row r="16" ht="15.75" customHeight="1" spans="1:14">
       <c r="A16" s="25" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
@@ -11490,7 +11500,7 @@
     </row>
     <row r="17" ht="15.75" customHeight="1" spans="1:14">
       <c r="A17" s="25" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>15</v>
@@ -11522,7 +11532,7 @@
     </row>
     <row r="18" ht="15.75" customHeight="1" spans="1:14">
       <c r="A18" s="25" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
@@ -11542,7 +11552,7 @@
     </row>
     <row r="19" ht="15.75" customHeight="1" spans="1:14">
       <c r="A19" s="31" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B19" s="29"/>
       <c r="C19" s="26">
@@ -11574,7 +11584,7 @@
     </row>
     <row r="20" ht="15.75" customHeight="1" spans="1:14">
       <c r="A20" s="25" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B20" s="29"/>
       <c r="C20" s="26">
@@ -11606,7 +11616,7 @@
     </row>
     <row r="21" ht="15.75" customHeight="1" spans="1:14">
       <c r="A21" s="25" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B21" s="29"/>
       <c r="C21" s="32"/>
@@ -11626,10 +11636,10 @@
     </row>
     <row r="22" ht="15.75" customHeight="1" spans="1:14">
       <c r="A22" s="25" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="B22" s="25" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C22" s="26">
         <v>9</v>
@@ -11660,7 +11670,7 @@
     </row>
     <row r="23" ht="15.75" customHeight="1" spans="1:14">
       <c r="A23" s="25" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B23" s="29"/>
       <c r="C23" s="26">
@@ -11690,7 +11700,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1" spans="1:14">
       <c r="A24" s="25" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
@@ -11718,7 +11728,7 @@
     </row>
     <row r="25" ht="15.75" customHeight="1" spans="1:14">
       <c r="A25" s="25" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="B25" s="29"/>
       <c r="C25" s="29"/>
@@ -11746,7 +11756,7 @@
     </row>
     <row r="26" ht="15.75" customHeight="1" spans="1:14">
       <c r="A26" s="25" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B26" s="29"/>
       <c r="C26" s="29"/>
@@ -11774,10 +11784,10 @@
     </row>
     <row r="27" ht="15.75" customHeight="1" spans="1:14">
       <c r="A27" s="25" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B27" s="25" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="C27" s="26">
         <v>13</v>
@@ -11806,7 +11816,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1" spans="1:14">
       <c r="A28" s="25" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
@@ -11834,7 +11844,7 @@
     </row>
     <row r="29" ht="15.75" customHeight="1" spans="1:14">
       <c r="A29" s="25" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
@@ -11862,7 +11872,7 @@
     </row>
     <row r="30" ht="15.75" customHeight="1" spans="1:14">
       <c r="A30" s="25" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
@@ -11890,7 +11900,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1" spans="1:14">
       <c r="A31" s="25" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
@@ -11918,7 +11928,7 @@
     </row>
     <row r="32" ht="15.75" customHeight="1" spans="1:14">
       <c r="A32" s="25" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
@@ -11971,49 +11981,49 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:28">
       <c r="A1" s="1" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="4"/>
       <c r="I1" s="5" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="8" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
       <c r="P1" s="8"/>
       <c r="Q1" s="9" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="R1" s="9"/>
       <c r="S1" s="9"/>
       <c r="T1" s="9"/>
       <c r="U1" s="10" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="V1" s="10"/>
       <c r="W1" s="10"/>
       <c r="X1" s="10"/>
       <c r="Y1" s="9" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="Z1" s="9"/>
       <c r="AA1" s="9"/>
@@ -12021,99 +12031,99 @@
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:28">
       <c r="A2" s="1" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="U2" s="11" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="V2" s="11" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="W2" s="11" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="X2" s="11" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="Z2" s="7" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="AA2" s="7" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="AB2" s="7" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" spans="1:28">
       <c r="A3" s="12" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>332</v>
@@ -12193,16 +12203,16 @@
     </row>
     <row r="4" ht="15.75" customHeight="1" spans="1:28">
       <c r="A4" s="12" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>22</v>
@@ -12279,16 +12289,16 @@
     </row>
     <row r="5" ht="15.75" customHeight="1" spans="1:28">
       <c r="A5" s="12" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>22</v>
@@ -12365,16 +12375,16 @@
     </row>
     <row r="6" ht="15.75" customHeight="1" spans="1:28">
       <c r="A6" s="12" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>22</v>
@@ -12451,16 +12461,16 @@
     </row>
     <row r="7" ht="15.75" customHeight="1" spans="1:28">
       <c r="A7" s="12" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>22</v>
@@ -12537,13 +12547,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1" spans="1:28">
       <c r="A8" s="12" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>334</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>332</v>
@@ -12621,16 +12631,16 @@
     </row>
     <row r="9" ht="15.75" customHeight="1" spans="1:28">
       <c r="A9" s="15" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>334</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="E9" s="17" t="s">
         <v>31</v>
@@ -12707,16 +12717,16 @@
     </row>
     <row r="10" ht="15.75" customHeight="1" spans="1:28">
       <c r="A10" s="12" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>334</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>22</v>
@@ -12793,16 +12803,16 @@
     </row>
     <row r="11" ht="15.75" customHeight="1" spans="1:28">
       <c r="A11" s="12" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>334</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="E11" s="14" t="s">
         <v>22</v>
@@ -12879,16 +12889,16 @@
     </row>
     <row r="12" ht="15.75" customHeight="1" spans="1:28">
       <c r="A12" s="12" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>332</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>22</v>
@@ -12965,16 +12975,16 @@
     </row>
     <row r="13" ht="15.75" customHeight="1" spans="1:28">
       <c r="A13" s="12" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>332</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>22</v>
@@ -13057,7 +13067,7 @@
         <v>39</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>332</v>
@@ -13143,10 +13153,10 @@
         <v>39</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>22</v>
@@ -13229,10 +13239,10 @@
         <v>39</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>22</v>
@@ -13315,10 +13325,10 @@
         <v>39</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>22</v>

</xml_diff>